<commit_message>
contest 2 dc vs kxi
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA56F674-A3C0-8349-B330-713658769A89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DE6663-3F36-3249-81E5-F22240AE58B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="3240" yWindow="1960" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Points</t>
   </si>
@@ -102,13 +102,31 @@
   </si>
   <si>
     <t>KKR vs SRH</t>
+  </si>
+  <si>
+    <t>JUSTIN CHALLENGERS</t>
+  </si>
+  <si>
+    <t>Garuda Tejas</t>
+  </si>
+  <si>
+    <t>Jais Royal Challengers</t>
+  </si>
+  <si>
+    <t>SUSHVIS CHOSEN ONES</t>
+  </si>
+  <si>
+    <t>GHOST RIDERS 6934</t>
+  </si>
+  <si>
+    <t>Anantha Team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,8 +150,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +181,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -220,10 +251,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -239,161 +271,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -948,6 +834,32 @@
         <v>-25</v>
       </c>
     </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="J8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="15"/>
+      <c r="M8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="P8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="15"/>
+      <c r="S8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="15"/>
+    </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>2</v>
@@ -1058,36 +970,48 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="D11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="G11" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E11" s="1">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="J11" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H11" s="1">
+        <v>60</v>
+      </c>
+      <c r="J11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="M11" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1">
+        <v>80</v>
+      </c>
+      <c r="M11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="P11" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N11" s="1">
+        <v>100</v>
+      </c>
+      <c r="P11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q11" s="1"/>
-      <c r="S11" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>40</v>
+      </c>
+      <c r="S11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T11" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1448,42 +1372,42 @@
       </c>
       <c r="E22" s="12">
         <f>SUM(D10:D17)</f>
-        <v>-15</v>
+        <v>-35</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="12">
         <f>SUM(G10:G17)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K22" s="12">
         <f>SUM(J10:J17)</f>
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="M22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N22" s="12">
         <f>SUM(M10:M17)</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="P22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q22" s="12">
         <f>SUM(P10:P17)</f>
-        <v>-20</v>
+        <v>-35</v>
       </c>
       <c r="S22" s="7" t="s">
         <v>13</v>
       </c>
       <c r="T22" s="12">
         <f>SUM(S10:S17)</f>
-        <v>-25</v>
+        <v>-50</v>
       </c>
       <c r="U22" s="1">
         <f>SUM(E22,H22,K22,N22,Q22,T22)</f>
@@ -1519,25 +1443,33 @@
       <c r="E26" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="S8:T8"/>
+  </mergeCells>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="31" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="32" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
contest 3 srh vs rcb
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DE6663-3F36-3249-81E5-F22240AE58B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F692CB44-390C-3B44-9070-DEE24FB5823A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="1960" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Points</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Anantha Team</t>
+  </si>
+  <si>
+    <t>RR vs KXI</t>
+  </si>
+  <si>
+    <t>RCB vs MI</t>
   </si>
 </sst>
 </file>
@@ -770,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15:S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,36 +1029,48 @@
       <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3" t="str">
+      <c r="D12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="G12" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E12" s="1">
+        <v>20</v>
+      </c>
+      <c r="G12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="J12" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
+        <v>80</v>
+      </c>
+      <c r="J12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="M12" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K12" s="1">
+        <v>40</v>
+      </c>
+      <c r="M12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="P12" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N12" s="1">
+        <v>60</v>
+      </c>
+      <c r="P12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q12" s="1"/>
-      <c r="S12" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>100</v>
+      </c>
+      <c r="S12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T12" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1266,167 +1284,235 @@
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
+      <c r="C18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E18" s="4"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H18" s="4"/>
-      <c r="J18" s="14"/>
+      <c r="J18" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K18" s="4"/>
-      <c r="M18" s="14"/>
+      <c r="M18" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N18" s="4"/>
-      <c r="P18" s="14"/>
+      <c r="P18" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q18" s="4"/>
-      <c r="S18" s="14"/>
+      <c r="S18" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T18" s="4"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="1">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="J19" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="M19" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N19" s="4"/>
-      <c r="P19" s="4"/>
+      <c r="P19" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q19" s="4"/>
-      <c r="S19" s="4"/>
+      <c r="S19" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T19" s="4"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="1" t="s">
+      <c r="A20" s="1">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="4"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="4"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="4"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="4"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="4"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="4"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="9" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="9" t="s">
+      <c r="G22" s="1"/>
+      <c r="H22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="9" t="s">
+      <c r="J22" s="1"/>
+      <c r="K22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="1"/>
-      <c r="N20" s="9" t="s">
+      <c r="M22" s="1"/>
+      <c r="N22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="9" t="s">
+      <c r="P22" s="1"/>
+      <c r="Q22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S20" s="1"/>
-      <c r="T20" s="9" t="s">
+      <c r="S22" s="1"/>
+      <c r="T22" s="9" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M21" s="1"/>
-      <c r="N21" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S21" s="1"/>
-      <c r="T21" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="12">
-        <f>SUM(D10:D17)</f>
-        <v>-35</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="12">
-        <f>SUM(G10:G17)</f>
-        <v>10</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="12">
-        <f>SUM(J10:J17)</f>
-        <v>10</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N22" s="12">
-        <f>SUM(M10:M17)</f>
-        <v>100</v>
-      </c>
-      <c r="P22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q22" s="12">
-        <f>SUM(P10:P17)</f>
-        <v>-35</v>
-      </c>
-      <c r="S22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T22" s="12">
-        <f>SUM(S10:S17)</f>
-        <v>-50</v>
-      </c>
-      <c r="U22" s="1">
-        <f>SUM(E22,H22,K22,N22,Q22,T22)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D23" s="1"/>
+      <c r="E23" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S23" s="1"/>
+      <c r="T23" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="D24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="12">
+        <f>SUM(D10:D17)</f>
+        <v>-55</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="12">
+        <f>SUM(G10:G17)</f>
+        <v>30</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="12">
+        <f>SUM(J10:J17)</f>
+        <v>-5</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N24" s="12">
+        <f>SUM(M10:M17)</f>
+        <v>90</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q24" s="12">
+        <f>SUM(P10:P17)</f>
+        <v>15</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T24" s="12">
+        <f>SUM(S10:S17)</f>
+        <v>-75</v>
+      </c>
+      <c r="U24" s="1">
+        <f>SUM(E24,H24,K24,N24,Q24,T24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
@@ -1441,6 +1527,20 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1451,7 +1551,7 @@
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="S8:T8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E24">
     <cfRule type="cellIs" dxfId="17" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1462,7 +1562,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="H24">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1473,7 +1573,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
+  <conditionalFormatting sqref="K24">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1484,7 +1584,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N22">
+  <conditionalFormatting sqref="N24">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1495,7 +1595,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q22">
+  <conditionalFormatting sqref="Q24">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1506,7 +1606,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T22">
+  <conditionalFormatting sqref="T24">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
contest 5 kkr vs mi
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7E9E64-B8A2-7A47-8D02-CB46255B8FA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F513356-CF4E-374D-9622-3383AC98BBF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="1960" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2220" yWindow="1780" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Points</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>RR vs KKR</t>
+  </si>
+  <si>
+    <t>KXI vs MI</t>
   </si>
 </sst>
 </file>
@@ -782,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,36 +1144,48 @@
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="D14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="G14" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E14" s="1">
+        <v>60</v>
+      </c>
+      <c r="G14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="J14" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H14" s="1">
+        <v>100</v>
+      </c>
+      <c r="J14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="M14" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K14" s="1">
+        <v>20</v>
+      </c>
+      <c r="M14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="P14" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N14" s="1">
+        <v>40</v>
+      </c>
+      <c r="P14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="1"/>
-      <c r="S14" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>80</v>
+      </c>
+      <c r="S14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T14" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1454,145 +1469,161 @@
       <c r="T21" s="4"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="A22" s="1">
+        <v>13</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="14"/>
       <c r="E22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="14"/>
       <c r="H22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="14"/>
       <c r="K22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="M22" s="14"/>
       <c r="N22" s="4"/>
-      <c r="P22" s="4"/>
+      <c r="P22" s="14"/>
       <c r="Q22" s="4"/>
-      <c r="S22" s="4"/>
+      <c r="S22" s="14"/>
       <c r="T22" s="4"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="1" t="s">
+      <c r="A23" s="1"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="9" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="9" t="s">
+      <c r="G24" s="1"/>
+      <c r="H24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="9" t="s">
+      <c r="J24" s="1"/>
+      <c r="K24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="1"/>
-      <c r="N23" s="9" t="s">
+      <c r="M24" s="1"/>
+      <c r="N24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="9" t="s">
+      <c r="P24" s="1"/>
+      <c r="Q24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S23" s="1"/>
-      <c r="T23" s="9" t="s">
+      <c r="S24" s="1"/>
+      <c r="T24" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M24" s="1"/>
-      <c r="N24" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S24" s="1"/>
-      <c r="T24" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="12">
-        <f>SUM(D10:D17)</f>
-        <v>-75</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="12">
-        <f>SUM(G10:G17)</f>
-        <v>50</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K25" s="12">
-        <f>SUM(J10:J17)</f>
-        <v>-20</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N25" s="12">
-        <f>SUM(M10:M17)</f>
-        <v>140</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q25" s="12">
-        <f>SUM(P10:P17)</f>
-        <v>5</v>
-      </c>
-      <c r="S25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T25" s="12">
-        <f>SUM(S10:S17)</f>
-        <v>-100</v>
-      </c>
-      <c r="U25" s="1">
-        <f>SUM(E25,H25,K25,N25,Q25,T25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+      <c r="E25" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S25" s="1"/>
+      <c r="T25" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="D26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="12">
+        <f>SUM(D10:D17)</f>
+        <v>-85</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="12">
+        <f>SUM(G10:G17)</f>
+        <v>100</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="12">
+        <f>SUM(J10:J17)</f>
+        <v>-40</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="12">
+        <f>SUM(M10:M17)</f>
+        <v>125</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q26" s="12">
+        <f>SUM(P10:P17)</f>
+        <v>25</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T26" s="12">
+        <f>SUM(S10:S17)</f>
+        <v>-125</v>
+      </c>
+      <c r="U26" s="1">
+        <f>SUM(E26,H26,K26,N26,Q26,T26)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
@@ -1614,6 +1645,13 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1624,7 +1662,7 @@
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="S8:T8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E25">
+  <conditionalFormatting sqref="E26">
     <cfRule type="cellIs" dxfId="17" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1635,7 +1673,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
+  <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1646,7 +1684,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1657,7 +1695,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N25">
+  <conditionalFormatting sqref="N26">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1668,7 +1706,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q25">
+  <conditionalFormatting sqref="Q26">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1679,7 +1717,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T25">
+  <conditionalFormatting sqref="T26">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
contest 6 kxi vs rcb
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F513356-CF4E-374D-9622-3383AC98BBF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A36FDBF-F10C-A84B-8061-75FBB5B50245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1780" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="220" yWindow="640" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Points</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>KXI vs MI</t>
+  </si>
+  <si>
+    <t>CSK vs SRH</t>
   </si>
 </sst>
 </file>
@@ -785,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,36 +1200,48 @@
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="G15" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1">
+        <v>80</v>
+      </c>
+      <c r="G15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="J15" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H15" s="1">
+        <v>60</v>
+      </c>
+      <c r="J15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="M15" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K15" s="1">
+        <v>20</v>
+      </c>
+      <c r="M15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N15" s="1"/>
-      <c r="P15" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N15" s="1">
+        <v>40</v>
+      </c>
+      <c r="P15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="1"/>
-      <c r="S15" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T15" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="T15" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1478,7 +1493,10 @@
       <c r="C22" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="14"/>
+      <c r="D22" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E22" s="4"/>
       <c r="G22" s="14"/>
       <c r="H22" s="4"/>
@@ -1492,145 +1510,179 @@
       <c r="T22" s="4"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="A23" s="1">
+        <v>14</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="M23" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N23" s="4"/>
-      <c r="P23" s="4"/>
+      <c r="P23" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q23" s="4"/>
-      <c r="S23" s="4"/>
+      <c r="S23" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T23" s="4"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="9" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="9" t="s">
+      <c r="G25" s="1"/>
+      <c r="H25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="9" t="s">
+      <c r="J25" s="1"/>
+      <c r="K25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M24" s="1"/>
-      <c r="N24" s="9" t="s">
+      <c r="M25" s="1"/>
+      <c r="N25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="9" t="s">
+      <c r="P25" s="1"/>
+      <c r="Q25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S24" s="1"/>
-      <c r="T24" s="9" t="s">
+      <c r="S25" s="1"/>
+      <c r="T25" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M25" s="1"/>
-      <c r="N25" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S25" s="1"/>
-      <c r="T25" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="12">
-        <f>SUM(D10:D17)</f>
-        <v>-85</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="12">
-        <f>SUM(G10:G17)</f>
-        <v>100</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="12">
-        <f>SUM(J10:J17)</f>
-        <v>-40</v>
-      </c>
-      <c r="M26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N26" s="12">
-        <f>SUM(M10:M17)</f>
-        <v>125</v>
-      </c>
-      <c r="P26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q26" s="12">
-        <f>SUM(P10:P17)</f>
-        <v>25</v>
-      </c>
-      <c r="S26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T26" s="12">
-        <f>SUM(S10:S17)</f>
-        <v>-125</v>
-      </c>
-      <c r="U26" s="1">
-        <f>SUM(E26,H26,K26,N26,Q26,T26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D26" s="1"/>
+      <c r="E26" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S26" s="1"/>
+      <c r="T26" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="D27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="12">
+        <f>SUM(D10:D17)</f>
+        <v>-65</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="12">
+        <f>SUM(G10:G17)</f>
+        <v>90</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="12">
+        <f>SUM(J10:J17)</f>
+        <v>-60</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N27" s="12">
+        <f>SUM(M10:M17)</f>
+        <v>110</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q27" s="12">
+        <f>SUM(P10:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T27" s="12">
+        <f>SUM(S10:S17)</f>
+        <v>-75</v>
+      </c>
+      <c r="U27" s="1">
+        <f>SUM(E27,H27,K27,N27,Q27,T27)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
@@ -1653,16 +1705,23 @@
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="S8:T8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="S8:T8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E26">
+  <conditionalFormatting sqref="E27">
     <cfRule type="cellIs" dxfId="17" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1673,7 +1732,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1684,7 +1743,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K27">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1695,7 +1754,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
+  <conditionalFormatting sqref="N27">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1706,7 +1765,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q26">
+  <conditionalFormatting sqref="Q27">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1717,7 +1776,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T26">
+  <conditionalFormatting sqref="T27">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 10 rcb vs mi - super over and super win for rcb
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A36FDBF-F10C-A84B-8061-75FBB5B50245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB6A711-96D4-FB42-9F99-8F392A016BD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="640" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -25,18 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Points</t>
   </si>
@@ -138,13 +132,31 @@
   </si>
   <si>
     <t>CSK vs SRH</t>
+  </si>
+  <si>
+    <t>RCB vs RR</t>
+  </si>
+  <si>
+    <t>DC vs KKR</t>
+  </si>
+  <si>
+    <t>MI vs SRH</t>
+  </si>
+  <si>
+    <t>KXI vs CSK</t>
+  </si>
+  <si>
+    <t>RCB vs DC</t>
+  </si>
+  <si>
+    <t>AFA - DREAM 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +182,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="30"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -273,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -292,12 +312,195 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -788,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+      <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,6 +1014,15 @@
       <c r="B2" s="8">
         <v>50</v>
       </c>
+      <c r="I2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -819,6 +1031,13 @@
       <c r="B3" s="8">
         <v>20</v>
       </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
@@ -827,6 +1046,13 @@
       <c r="B4" s="8">
         <v>-10</v>
       </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
@@ -835,6 +1061,13 @@
       <c r="B5" s="8">
         <v>-15</v>
       </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
@@ -843,6 +1076,13 @@
       <c r="B6" s="8">
         <v>-20</v>
       </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
@@ -1253,38 +1493,50 @@
       <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="3" t="str">
+      <c r="D16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="G16" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>60</v>
+      </c>
+      <c r="G16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="J16" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
+        <v>80</v>
+      </c>
+      <c r="J16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="M16" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K16" s="1">
+        <v>100</v>
+      </c>
+      <c r="M16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N16" s="1"/>
-      <c r="P16" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N16" s="1">
+        <v>40</v>
+      </c>
+      <c r="P16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="1"/>
-      <c r="S16" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>20</v>
+      </c>
+      <c r="S16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T16" s="1"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-25</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -1294,38 +1546,50 @@
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="D17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="G17" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E17" s="1">
+        <v>40</v>
+      </c>
+      <c r="G17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="J17" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H17" s="1">
+        <v>20</v>
+      </c>
+      <c r="J17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="M17" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K17" s="1">
+        <v>60</v>
+      </c>
+      <c r="M17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N17" s="1"/>
-      <c r="P17" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N17" s="1">
+        <v>80</v>
+      </c>
+      <c r="P17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="1"/>
-      <c r="S17" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>100</v>
+      </c>
+      <c r="S17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-25</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -1335,38 +1599,50 @@
       <c r="C18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="D18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="G18" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E18" s="4">
+        <v>100</v>
+      </c>
+      <c r="G18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H18" s="4"/>
-      <c r="J18" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H18" s="4">
+        <v>40</v>
+      </c>
+      <c r="J18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K18" s="4"/>
-      <c r="M18" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K18" s="4">
+        <v>80</v>
+      </c>
+      <c r="M18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N18" s="4"/>
-      <c r="P18" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="4"/>
-      <c r="S18" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>60</v>
+      </c>
+      <c r="S18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T18" s="4"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-20</v>
+      </c>
+      <c r="T18" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -1376,38 +1652,50 @@
       <c r="C19" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="G19" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E19" s="4">
+        <v>80</v>
+      </c>
+      <c r="G19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H19" s="4"/>
-      <c r="J19" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H19" s="4">
+        <v>20</v>
+      </c>
+      <c r="J19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K19" s="4"/>
-      <c r="M19" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K19" s="4">
+        <v>40</v>
+      </c>
+      <c r="M19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N19" s="4"/>
-      <c r="P19" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N19" s="4">
+        <v>60</v>
+      </c>
+      <c r="P19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="4"/>
-      <c r="S19" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T19" s="4"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="T19" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -1445,7 +1733,7 @@
       </c>
       <c r="T20" s="4"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -1483,7 +1771,7 @@
       </c>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>13</v>
       </c>
@@ -1509,7 +1797,7 @@
       <c r="S22" s="14"/>
       <c r="T22" s="4"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>14</v>
       </c>
@@ -1550,170 +1838,411 @@
       </c>
       <c r="T23" s="4"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>15</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="G24" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="J24" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="M24" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N24" s="4"/>
-      <c r="P24" s="4"/>
+      <c r="P24" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q24" s="4"/>
-      <c r="S24" s="4"/>
+      <c r="S24" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="1" t="s">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>16</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="G25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="J25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K25" s="4"/>
+      <c r="M25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="P25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q25" s="4"/>
+      <c r="S25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T25" s="4"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>17</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="G26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="J26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K26" s="4"/>
+      <c r="M26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="P26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q26" s="4"/>
+      <c r="S26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T26" s="4"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>18</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="G27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="J27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="M27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N27" s="4"/>
+      <c r="P27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q27" s="4"/>
+      <c r="S27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T27" s="4"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>19</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="G28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="J28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="M28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="P28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q28" s="4"/>
+      <c r="S28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T28" s="4"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="G29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="J29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="M29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N29" s="4"/>
+      <c r="P29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q29" s="4"/>
+      <c r="S29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T29" s="4"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="9" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="9" t="s">
+      <c r="G31" s="1"/>
+      <c r="H31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="9" t="s">
+      <c r="J31" s="1"/>
+      <c r="K31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M25" s="1"/>
-      <c r="N25" s="9" t="s">
+      <c r="M31" s="1"/>
+      <c r="N31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="9" t="s">
+      <c r="P31" s="1"/>
+      <c r="Q31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S25" s="1"/>
-      <c r="T25" s="9" t="s">
+      <c r="S31" s="1"/>
+      <c r="T31" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="11" t="str">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="11" t="str">
         <f>D9</f>
         <v>Anantha</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="11" t="str">
+      <c r="G32" s="1"/>
+      <c r="H32" s="11" t="str">
         <f>G9</f>
         <v>Jayanth</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="11" t="str">
+      <c r="J32" s="1"/>
+      <c r="K32" s="11" t="str">
         <f>J9</f>
         <v>Justin</v>
       </c>
-      <c r="M26" s="1"/>
-      <c r="N26" s="11" t="str">
+      <c r="M32" s="1"/>
+      <c r="N32" s="11" t="str">
         <f>M9</f>
         <v>Rapaka</v>
       </c>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="11" t="str">
+      <c r="P32" s="1"/>
+      <c r="Q32" s="11" t="str">
         <f>P9</f>
         <v>Sushma</v>
       </c>
-      <c r="S26" s="1"/>
-      <c r="T26" s="11" t="str">
+      <c r="S32" s="1"/>
+      <c r="T32" s="11" t="str">
         <f>S9</f>
         <v>Sampath M</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="7" t="s">
+    <row r="33" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="12">
-        <f>SUM(D10:D17)</f>
-        <v>-65</v>
-      </c>
-      <c r="G27" s="7" t="s">
+      <c r="E33" s="12">
+        <f>SUM(D10:D29)</f>
+        <v>-20</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="12">
-        <f>SUM(G10:G17)</f>
-        <v>90</v>
-      </c>
-      <c r="J27" s="7" t="s">
+      <c r="H33" s="12">
+        <f>SUM(G10:G29)</f>
+        <v>55</v>
+      </c>
+      <c r="J33" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="12">
-        <f>SUM(J10:J17)</f>
-        <v>-60</v>
-      </c>
-      <c r="M27" s="7" t="s">
+      <c r="K33" s="12">
+        <f>SUM(J10:J29)</f>
+        <v>-15</v>
+      </c>
+      <c r="M33" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N27" s="12">
-        <f>SUM(M10:M17)</f>
-        <v>110</v>
-      </c>
-      <c r="P27" s="7" t="s">
+      <c r="N33" s="12">
+        <f>SUM(M10:M29)</f>
+        <v>80</v>
+      </c>
+      <c r="P33" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q27" s="12">
-        <f>SUM(P10:P17)</f>
+      <c r="Q33" s="12">
+        <f>SUM(P10:P29)</f>
+        <v>-5</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T33" s="12">
+        <f>SUM(S10:S29)</f>
+        <v>-95</v>
+      </c>
+      <c r="U33" s="1">
+        <f>SUM(E33,H33,K33,N33,Q33,T33)</f>
         <v>0</v>
       </c>
-      <c r="S27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T27" s="12">
-        <f>SUM(S10:S17)</f>
-        <v>-75</v>
-      </c>
-      <c r="U27" s="1">
-        <f>SUM(E27,H27,K27,N27,Q27,T27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="I2:O6"/>
     <mergeCell ref="S8:T8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:H8"/>
@@ -1721,29 +2250,40 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="17" priority="31" operator="lessThan">
+  <conditionalFormatting sqref="E33">
+    <cfRule type="cellIs" dxfId="35" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="51" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
+  <conditionalFormatting sqref="K33">
+    <cfRule type="cellIs" dxfId="32" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="H33">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N33">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1754,18 +2294,18 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N27">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="T33">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q27">
+  <conditionalFormatting sqref="Q33">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1776,17 +2316,6 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Contest 12 RR vs KKR.
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB6A711-96D4-FB42-9F99-8F392A016BD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBC5693-B531-8B40-AE73-8E688728B2EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="640" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="220" yWindow="620" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Points</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>AFA - DREAM 11</t>
+  </si>
+  <si>
+    <t>MI vs RR</t>
+  </si>
+  <si>
+    <t>KKR vs CSK</t>
   </si>
 </sst>
 </file>
@@ -196,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +231,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -293,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -308,11 +320,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -991,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+      <selection activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,15 +1025,15 @@
       <c r="B2" s="8">
         <v>50</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -1031,13 +1042,13 @@
       <c r="B3" s="8">
         <v>20</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
@@ -1046,13 +1057,13 @@
       <c r="B4" s="8">
         <v>-10</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
@@ -1061,13 +1072,13 @@
       <c r="B5" s="8">
         <v>-15</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
@@ -1076,13 +1087,13 @@
       <c r="B6" s="8">
         <v>-20</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
@@ -1093,30 +1104,30 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="G8" s="15" t="s">
+      <c r="E8" s="14"/>
+      <c r="G8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="J8" s="15" t="s">
+      <c r="H8" s="14"/>
+      <c r="J8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="M8" s="15" t="s">
+      <c r="K8" s="14"/>
+      <c r="M8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="15"/>
-      <c r="P8" s="15" t="s">
+      <c r="N8" s="14"/>
+      <c r="P8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="15"/>
-      <c r="S8" s="15" t="s">
+      <c r="Q8" s="14"/>
+      <c r="S8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="15"/>
+      <c r="T8" s="14"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
@@ -1705,33 +1716,48 @@
       <c r="C20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="D20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="G20" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H20" s="4"/>
-      <c r="J20" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H20" s="4">
+        <v>20</v>
+      </c>
+      <c r="J20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K20" s="4"/>
-      <c r="M20" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K20" s="4">
+        <v>100</v>
+      </c>
+      <c r="M20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N20" s="4"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="4"/>
-      <c r="S20" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N20" s="4">
+        <v>40</v>
+      </c>
+      <c r="P20" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>80</v>
+      </c>
+      <c r="S20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T20" s="4"/>
+        <v>-10</v>
+      </c>
+      <c r="T20" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1743,33 +1769,48 @@
       <c r="C21" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="3" t="str">
+      <c r="D21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="G21" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H21" s="4"/>
-      <c r="J21" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H21" s="4">
+        <v>100</v>
+      </c>
+      <c r="J21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K21" s="4"/>
-      <c r="M21" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K21" s="4">
+        <v>20</v>
+      </c>
+      <c r="M21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N21" s="4"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="4"/>
-      <c r="S21" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N21" s="4">
+        <v>80</v>
+      </c>
+      <c r="P21" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>60</v>
+      </c>
+      <c r="S21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T21" s="4"/>
+        <v>-15</v>
+      </c>
+      <c r="T21" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1786,15 +1827,30 @@
         <v/>
       </c>
       <c r="E22" s="4"/>
-      <c r="G22" s="14"/>
+      <c r="G22" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H22" s="4"/>
-      <c r="J22" s="14"/>
+      <c r="J22" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K22" s="4"/>
-      <c r="M22" s="14"/>
+      <c r="M22" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N22" s="4"/>
-      <c r="P22" s="14"/>
+      <c r="P22" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q22" s="4"/>
-      <c r="S22" s="14"/>
+      <c r="S22" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T22" s="4"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -2044,9 +2100,15 @@
       <c r="T28" s="4"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="13"/>
+      <c r="A29" s="1">
+        <v>20</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>40</v>
+      </c>
       <c r="D29" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2079,152 +2141,214 @@
       <c r="T29" s="4"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="A30" s="1">
+        <v>21</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="G30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N30" s="4"/>
-      <c r="P30" s="4"/>
+      <c r="P30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q30" s="4"/>
-      <c r="S30" s="4"/>
+      <c r="S30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T30" s="4"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="1"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="G31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H31" s="4"/>
+      <c r="J31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K31" s="4"/>
+      <c r="M31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="P31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q31" s="4"/>
+      <c r="S31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T31" s="4"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="9" t="s">
+      <c r="C33" s="10"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="9" t="s">
+      <c r="G33" s="1"/>
+      <c r="H33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="9" t="s">
+      <c r="J33" s="1"/>
+      <c r="K33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M31" s="1"/>
-      <c r="N31" s="9" t="s">
+      <c r="M33" s="1"/>
+      <c r="N33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="9" t="s">
+      <c r="P33" s="1"/>
+      <c r="Q33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S31" s="1"/>
-      <c r="T31" s="9" t="s">
+      <c r="S33" s="1"/>
+      <c r="T33" s="9" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J32" s="1"/>
-      <c r="K32" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M32" s="1"/>
-      <c r="N32" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S32" s="1"/>
-      <c r="T32" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="12">
-        <f>SUM(D10:D29)</f>
-        <v>-20</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="12">
-        <f>SUM(G10:G29)</f>
-        <v>55</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="12">
-        <f>SUM(J10:J29)</f>
-        <v>-15</v>
-      </c>
-      <c r="M33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N33" s="12">
-        <f>SUM(M10:M29)</f>
-        <v>80</v>
-      </c>
-      <c r="P33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q33" s="12">
-        <f>SUM(P10:P29)</f>
-        <v>-5</v>
-      </c>
-      <c r="S33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T33" s="12">
-        <f>SUM(S10:S29)</f>
-        <v>-95</v>
-      </c>
-      <c r="U33" s="1">
-        <f>SUM(E33,H33,K33,N33,Q33,T33)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D34" s="1"/>
+      <c r="E34" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S34" s="1"/>
+      <c r="T34" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="D35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="12">
+        <f>SUM(D10:D31)</f>
+        <v>-70</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="12">
+        <f>SUM(G10:G31)</f>
+        <v>85</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="12">
+        <f>SUM(J10:J31)</f>
+        <v>15</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N35" s="12">
+        <f>SUM(M10:M31)</f>
+        <v>85</v>
+      </c>
+      <c r="P35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q35" s="12">
+        <f>SUM(P10:P31)</f>
+        <v>5</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T35" s="12">
+        <f>SUM(S10:S31)</f>
+        <v>-120</v>
+      </c>
+      <c r="U35" s="1">
+        <f>SUM(E35,H35,K35,N35,Q35,T35)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
@@ -2239,6 +2363,20 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2250,7 +2388,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E33">
+  <conditionalFormatting sqref="E35">
     <cfRule type="cellIs" dxfId="35" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2261,7 +2399,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K35">
     <cfRule type="cellIs" dxfId="32" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2272,7 +2410,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="20" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2283,7 +2421,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N33">
+  <conditionalFormatting sqref="N35">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2294,7 +2432,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T33">
+  <conditionalFormatting sqref="T35">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2305,7 +2443,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q33">
+  <conditionalFormatting sqref="Q35">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
contest 13 KXI vs MI.
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBC5693-B531-8B40-AE73-8E688728B2EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCCDF73-C055-6646-83F3-47EE3FA43878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="620" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>Points</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>KKR vs CSK</t>
+  </si>
+  <si>
+    <t>SRH vs KXI</t>
   </si>
 </sst>
 </file>
@@ -1002,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U35" sqref="U35"/>
+      <selection activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1822,36 +1825,46 @@
       <c r="C22" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="G22" s="3" t="str">
+      <c r="D22" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>20</v>
+      </c>
+      <c r="G22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H22" s="4"/>
-      <c r="J22" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H22" s="4">
+        <v>60</v>
+      </c>
+      <c r="J22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K22" s="4"/>
-      <c r="M22" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K22" s="4">
+        <v>40</v>
+      </c>
+      <c r="M22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N22" s="4"/>
-      <c r="P22" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N22" s="4">
+        <v>80</v>
+      </c>
+      <c r="P22" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q22" s="4"/>
-      <c r="S22" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T22" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>100</v>
+      </c>
+      <c r="S22" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="T22" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -2182,9 +2195,15 @@
       <c r="T30" s="4"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="13"/>
+      <c r="A31" s="1">
+        <v>22</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="D31" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2219,143 +2238,171 @@
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="G32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="J32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="M32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N32" s="4"/>
-      <c r="P32" s="4"/>
+      <c r="P32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q32" s="4"/>
-      <c r="S32" s="4"/>
+      <c r="S32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T32" s="4"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="1" t="s">
+      <c r="A33" s="1"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="9" t="s">
+      <c r="C34" s="10"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="9" t="s">
+      <c r="G34" s="1"/>
+      <c r="H34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="9" t="s">
+      <c r="J34" s="1"/>
+      <c r="K34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M33" s="1"/>
-      <c r="N33" s="9" t="s">
+      <c r="M34" s="1"/>
+      <c r="N34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="9" t="s">
+      <c r="P34" s="1"/>
+      <c r="Q34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S33" s="1"/>
-      <c r="T33" s="9" t="s">
+      <c r="S34" s="1"/>
+      <c r="T34" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S34" s="1"/>
-      <c r="T34" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="12">
-        <f>SUM(D10:D31)</f>
-        <v>-70</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="12">
-        <f>SUM(G10:G31)</f>
-        <v>85</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K35" s="12">
-        <f>SUM(J10:J31)</f>
-        <v>15</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N35" s="12">
-        <f>SUM(M10:M31)</f>
-        <v>85</v>
-      </c>
-      <c r="P35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q35" s="12">
-        <f>SUM(P10:P31)</f>
-        <v>5</v>
-      </c>
-      <c r="S35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T35" s="12">
-        <f>SUM(S10:S31)</f>
-        <v>-120</v>
-      </c>
-      <c r="U35" s="1">
-        <f>SUM(E35,H35,K35,N35,Q35,T35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D35" s="1"/>
+      <c r="E35" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M35" s="1"/>
+      <c r="N35" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S35" s="1"/>
+      <c r="T35" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="D36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="12">
+        <f>SUM(D10:D32)</f>
+        <v>-92.5</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="12">
+        <f>SUM(G10:G32)</f>
+        <v>75</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="12">
+        <f>SUM(J10:J32)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N36" s="12">
+        <f>SUM(M10:M32)</f>
+        <v>105</v>
+      </c>
+      <c r="P36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q36" s="12">
+        <f>SUM(P10:P32)</f>
+        <v>55</v>
+      </c>
+      <c r="S36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T36" s="12">
+        <f>SUM(S10:S32)</f>
+        <v>-142.5</v>
+      </c>
+      <c r="U36" s="1">
+        <f>SUM(E36,H36,K36,N36,Q36,T36)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
@@ -2377,6 +2424,13 @@
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2388,7 +2442,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E35">
+  <conditionalFormatting sqref="E36">
     <cfRule type="cellIs" dxfId="35" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2399,7 +2453,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
+  <conditionalFormatting sqref="K36">
     <cfRule type="cellIs" dxfId="32" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2410,7 +2464,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H36">
     <cfRule type="cellIs" dxfId="20" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2421,7 +2475,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N35">
+  <conditionalFormatting sqref="N36">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2432,7 +2486,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T35">
+  <conditionalFormatting sqref="T36">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2443,7 +2497,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q35">
+  <conditionalFormatting sqref="Q36">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 17 MI vs SRH and Contest 18 KXI vs CSK
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCCDF73-C055-6646-83F3-47EE3FA43878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201ACDA0-5A91-244C-9BD3-8F5F6F83E1FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="620" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="1460" yWindow="2240" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Points</t>
   </si>
@@ -159,6 +159,21 @@
   </si>
   <si>
     <t>SRH vs KXI</t>
+  </si>
+  <si>
+    <t>RR vs DC</t>
+  </si>
+  <si>
+    <t>KXI vs KKR</t>
+  </si>
+  <si>
+    <t>CSK vs RCB</t>
+  </si>
+  <si>
+    <t>SRH vs RR</t>
+  </si>
+  <si>
+    <t>MI vs DC</t>
   </si>
 </sst>
 </file>
@@ -323,198 +338,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1005,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U40"/>
+  <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U36" sqref="U36"/>
+      <selection activeCell="U41" sqref="U41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,15 +863,15 @@
       <c r="B2" s="8">
         <v>50</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -1045,13 +880,13 @@
       <c r="B3" s="8">
         <v>20</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
@@ -1060,13 +895,13 @@
       <c r="B4" s="8">
         <v>-10</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
@@ -1075,13 +910,13 @@
       <c r="B5" s="8">
         <v>-15</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
@@ -1090,13 +925,13 @@
       <c r="B6" s="8">
         <v>-20</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
@@ -1107,30 +942,30 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="G8" s="14" t="s">
+      <c r="E8" s="15"/>
+      <c r="G8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="J8" s="14" t="s">
+      <c r="H8" s="15"/>
+      <c r="J8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="M8" s="14" t="s">
+      <c r="K8" s="15"/>
+      <c r="M8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="14"/>
-      <c r="P8" s="14" t="s">
+      <c r="N8" s="15"/>
+      <c r="P8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="14"/>
-      <c r="S8" s="14" t="s">
+      <c r="Q8" s="15"/>
+      <c r="S8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="14"/>
+      <c r="T8" s="15"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
@@ -1876,36 +1711,48 @@
       <c r="C23" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="3" t="str">
+      <c r="D23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="G23" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E23" s="4">
+        <v>100</v>
+      </c>
+      <c r="G23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="J23" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H23" s="4">
+        <v>60</v>
+      </c>
+      <c r="J23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K23" s="4"/>
-      <c r="M23" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K23" s="4">
+        <v>80</v>
+      </c>
+      <c r="M23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N23" s="4"/>
-      <c r="P23" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N23" s="4">
+        <v>40</v>
+      </c>
+      <c r="P23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q23" s="4"/>
-      <c r="S23" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>20</v>
+      </c>
+      <c r="S23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T23" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T23" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1917,36 +1764,48 @@
       <c r="C24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="3" t="str">
+      <c r="D24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="G24" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E24" s="4">
+        <v>60</v>
+      </c>
+      <c r="G24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H24" s="4"/>
-      <c r="J24" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H24" s="4">
+        <v>80</v>
+      </c>
+      <c r="J24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K24" s="4"/>
-      <c r="M24" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K24" s="4">
+        <v>100</v>
+      </c>
+      <c r="M24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N24" s="4"/>
-      <c r="P24" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N24" s="4">
+        <v>40</v>
+      </c>
+      <c r="P24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q24" s="4"/>
-      <c r="S24" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>0</v>
+      </c>
+      <c r="S24" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T24" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T24" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1958,36 +1817,48 @@
       <c r="C25" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="3" t="str">
+      <c r="D25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="G25" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E25" s="4">
+        <v>40</v>
+      </c>
+      <c r="G25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H25" s="4"/>
-      <c r="J25" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H25" s="4">
+        <v>100</v>
+      </c>
+      <c r="J25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K25" s="4"/>
-      <c r="M25" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+      <c r="M25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N25" s="4"/>
-      <c r="P25" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N25" s="4">
+        <v>60</v>
+      </c>
+      <c r="P25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q25" s="4"/>
-      <c r="S25" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>80</v>
+      </c>
+      <c r="S25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T25" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T25" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1999,36 +1870,48 @@
       <c r="C26" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="3" t="str">
+      <c r="D26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="G26" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4">
+        <v>100</v>
+      </c>
+      <c r="G26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H26" s="4"/>
-      <c r="J26" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K26" s="4"/>
-      <c r="M26" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K26" s="4">
+        <v>60</v>
+      </c>
+      <c r="M26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N26" s="4"/>
-      <c r="P26" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N26" s="4">
+        <v>80</v>
+      </c>
+      <c r="P26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q26" s="4"/>
-      <c r="S26" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>20</v>
+      </c>
+      <c r="S26" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T26" s="4"/>
+        <v>-15</v>
+      </c>
+      <c r="T26" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -2040,36 +1923,48 @@
       <c r="C27" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="3" t="str">
+      <c r="D27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="G27" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4">
+        <v>100</v>
+      </c>
+      <c r="G27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="J27" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H27" s="4">
+        <v>80</v>
+      </c>
+      <c r="J27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K27" s="4"/>
-      <c r="M27" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K27" s="4">
+        <v>60</v>
+      </c>
+      <c r="M27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N27" s="4"/>
-      <c r="P27" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N27" s="4">
+        <v>20</v>
+      </c>
+      <c r="P27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q27" s="4"/>
-      <c r="S27" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>40</v>
+      </c>
+      <c r="S27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T27" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T27" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -2236,9 +2131,15 @@
       <c r="T31" s="4"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="13"/>
+      <c r="A32" s="1">
+        <v>23</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="D32" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2271,166 +2172,365 @@
       <c r="T32" s="4"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="A33" s="1">
+        <v>24</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="G33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="J33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="M33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N33" s="4"/>
-      <c r="P33" s="4"/>
+      <c r="P33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q33" s="4"/>
-      <c r="S33" s="4"/>
+      <c r="S33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T33" s="4"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A34" s="6"/>
-      <c r="B34" s="1" t="s">
+      <c r="A34" s="1">
+        <v>25</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="G34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="J34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K34" s="4"/>
+      <c r="M34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N34" s="4"/>
+      <c r="P34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q34" s="4"/>
+      <c r="S34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T34" s="4"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>26</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="G35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="J35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K35" s="4"/>
+      <c r="M35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N35" s="4"/>
+      <c r="P35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q35" s="4"/>
+      <c r="S35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T35" s="4"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>27</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="G36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="J36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K36" s="4"/>
+      <c r="M36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N36" s="4"/>
+      <c r="P36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q36" s="4"/>
+      <c r="S36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T36" s="4"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="G37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="J37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K37" s="4"/>
+      <c r="M37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N37" s="4"/>
+      <c r="P37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q37" s="4"/>
+      <c r="S37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T37" s="4"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="9" t="s">
+      <c r="C39" s="10"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="9" t="s">
+      <c r="G39" s="1"/>
+      <c r="H39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J34" s="1"/>
-      <c r="K34" s="9" t="s">
+      <c r="J39" s="1"/>
+      <c r="K39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="9" t="s">
+      <c r="M39" s="1"/>
+      <c r="N39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="9" t="s">
+      <c r="P39" s="1"/>
+      <c r="Q39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S34" s="1"/>
-      <c r="T34" s="9" t="s">
+      <c r="S39" s="1"/>
+      <c r="T39" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J35" s="1"/>
-      <c r="K35" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M35" s="1"/>
-      <c r="N35" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S35" s="1"/>
-      <c r="T35" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="12">
-        <f>SUM(D10:D32)</f>
-        <v>-92.5</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="12">
-        <f>SUM(G10:G32)</f>
-        <v>75</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K36" s="12">
-        <f>SUM(J10:J32)</f>
-        <v>0</v>
-      </c>
-      <c r="M36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N36" s="12">
-        <f>SUM(M10:M32)</f>
-        <v>105</v>
-      </c>
-      <c r="P36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q36" s="12">
-        <f>SUM(P10:P32)</f>
-        <v>55</v>
-      </c>
-      <c r="S36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T36" s="12">
-        <f>SUM(S10:S32)</f>
-        <v>-142.5</v>
-      </c>
-      <c r="U36" s="1">
-        <f>SUM(E36,H36,K36,N36,Q36,T36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J40" s="1"/>
+      <c r="K40" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S40" s="1"/>
+      <c r="T40" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="12">
+        <f>SUM(D10:D37)</f>
+        <v>32.5</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="12">
+        <f>SUM(G10:G37)</f>
+        <v>130</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K41" s="12">
+        <f>SUM(J10:J37)</f>
+        <v>25</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N41" s="12">
+        <f>SUM(M10:M37)</f>
+        <v>65</v>
+      </c>
+      <c r="P41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q41" s="12">
+        <f>SUM(P10:P37)</f>
+        <v>-5</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T41" s="12">
+        <f>SUM(S10:S37)</f>
+        <v>-247.5</v>
+      </c>
+      <c r="U41" s="1">
+        <f>SUM(E41,H41,K41,N41,Q41,T41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2442,69 +2542,69 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="35" priority="49" operator="lessThan">
+  <conditionalFormatting sqref="E41">
+    <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="51" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
-    <cfRule type="cellIs" dxfId="32" priority="13" operator="lessThan">
+  <conditionalFormatting sqref="K41">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="lessThan">
+  <conditionalFormatting sqref="H41">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N36">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
+  <conditionalFormatting sqref="N41">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T36">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="T41">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q36">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="Q41">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Contest 19 RCB vs DC
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201ACDA0-5A91-244C-9BD3-8F5F6F83E1FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2742254F-0B55-B548-B876-CB25F2DE4974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1460" yWindow="2240" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Points</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>MI vs DC</t>
+  </si>
+  <si>
+    <t>RCB vs KKR</t>
   </si>
 </sst>
 </file>
@@ -840,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U41" sqref="U41"/>
+      <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1976,36 +1979,48 @@
       <c r="C28" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="3" t="str">
+      <c r="D28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="G28" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E28" s="4">
+        <v>100</v>
+      </c>
+      <c r="G28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H28" s="4"/>
-      <c r="J28" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H28" s="4">
+        <v>60</v>
+      </c>
+      <c r="J28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K28" s="4"/>
-      <c r="M28" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K28" s="4">
+        <v>40</v>
+      </c>
+      <c r="M28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N28" s="4"/>
-      <c r="P28" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N28" s="4">
+        <v>80</v>
+      </c>
+      <c r="P28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q28" s="4"/>
-      <c r="S28" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>0</v>
+      </c>
+      <c r="S28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T28" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T28" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -2336,9 +2351,15 @@
       <c r="T36" s="4"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="13"/>
+      <c r="A37" s="1">
+        <v>28</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="D37" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2373,143 +2394,171 @@
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="G38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="J38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K38" s="4"/>
-      <c r="M38" s="4"/>
+      <c r="M38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N38" s="4"/>
-      <c r="P38" s="4"/>
+      <c r="P38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q38" s="4"/>
-      <c r="S38" s="4"/>
+      <c r="S38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T38" s="4"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="6"/>
-      <c r="B39" s="1" t="s">
+      <c r="A39" s="1"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="9" t="s">
+      <c r="C40" s="10"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="9" t="s">
+      <c r="G40" s="1"/>
+      <c r="H40" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J39" s="1"/>
-      <c r="K39" s="9" t="s">
+      <c r="J40" s="1"/>
+      <c r="K40" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M39" s="1"/>
-      <c r="N39" s="9" t="s">
+      <c r="M40" s="1"/>
+      <c r="N40" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="9" t="s">
+      <c r="P40" s="1"/>
+      <c r="Q40" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S39" s="1"/>
-      <c r="T39" s="9" t="s">
+      <c r="S40" s="1"/>
+      <c r="T40" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J40" s="1"/>
-      <c r="K40" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M40" s="1"/>
-      <c r="N40" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S40" s="1"/>
-      <c r="T40" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="D41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="12">
-        <f>SUM(D10:D37)</f>
-        <v>32.5</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="12">
-        <f>SUM(G10:G37)</f>
-        <v>130</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" s="12">
-        <f>SUM(J10:J37)</f>
-        <v>25</v>
-      </c>
-      <c r="M41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N41" s="12">
-        <f>SUM(M10:M37)</f>
-        <v>65</v>
-      </c>
-      <c r="P41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q41" s="12">
-        <f>SUM(P10:P37)</f>
-        <v>-5</v>
-      </c>
-      <c r="S41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T41" s="12">
-        <f>SUM(S10:S37)</f>
-        <v>-247.5</v>
-      </c>
-      <c r="U41" s="1">
-        <f>SUM(E41,H41,K41,N41,Q41,T41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D41" s="1"/>
+      <c r="E41" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J41" s="1"/>
+      <c r="K41" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M41" s="1"/>
+      <c r="N41" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S41" s="1"/>
+      <c r="T41" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="D42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="12">
+        <f>SUM(D10:D38)</f>
+        <v>82.5</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="12">
+        <f>SUM(G10:G38)</f>
+        <v>120</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" s="12">
+        <f>SUM(J10:J38)</f>
+        <v>10</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N42" s="12">
+        <f>SUM(M10:M38)</f>
+        <v>85</v>
+      </c>
+      <c r="P42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q42" s="12">
+        <f>SUM(P10:P38)</f>
+        <v>-30</v>
+      </c>
+      <c r="S42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T42" s="12">
+        <f>SUM(S10:S38)</f>
+        <v>-267.5</v>
+      </c>
+      <c r="U42" s="1">
+        <f>SUM(E42,H42,K42,N42,Q42,T42)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
@@ -2531,6 +2580,13 @@
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2542,7 +2598,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E41">
+  <conditionalFormatting sqref="E42">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2553,7 +2609,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41">
+  <conditionalFormatting sqref="K42">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2564,7 +2620,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
+  <conditionalFormatting sqref="H42">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2575,7 +2631,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N41">
+  <conditionalFormatting sqref="N42">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2586,7 +2642,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T41">
+  <conditionalFormatting sqref="T42">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2597,7 +2653,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q41">
+  <conditionalFormatting sqref="Q42">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 20 MI vs RR
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2742254F-0B55-B548-B876-CB25F2DE4974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65DBA3E-A983-4A4D-B84F-54E80713B26F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1460" yWindow="2240" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Points</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>RCB vs KKR</t>
+  </si>
+  <si>
+    <t>SRH vs CSK</t>
   </si>
 </sst>
 </file>
@@ -843,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U46"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U42" sqref="U42"/>
+      <selection activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2032,36 +2035,48 @@
       <c r="C29" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="3" t="str">
+      <c r="D29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="G29" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="J29" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H29" s="4">
+        <v>100</v>
+      </c>
+      <c r="J29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K29" s="4"/>
-      <c r="M29" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K29" s="4">
+        <v>40</v>
+      </c>
+      <c r="M29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N29" s="4"/>
-      <c r="P29" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N29" s="4">
+        <v>60</v>
+      </c>
+      <c r="P29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q29" s="4"/>
-      <c r="S29" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>80</v>
+      </c>
+      <c r="S29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T29" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T29" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -2392,9 +2407,15 @@
       <c r="T37" s="4"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="13"/>
+      <c r="A38" s="1">
+        <v>29</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="D38" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2429,143 +2450,171 @@
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="G39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="J39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="M39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N39" s="4"/>
-      <c r="P39" s="4"/>
+      <c r="P39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q39" s="4"/>
-      <c r="S39" s="4"/>
+      <c r="S39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="6"/>
-      <c r="B40" s="1" t="s">
+      <c r="A40" s="1"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="9" t="s">
+      <c r="C41" s="10"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="9" t="s">
+      <c r="G41" s="1"/>
+      <c r="H41" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J40" s="1"/>
-      <c r="K40" s="9" t="s">
+      <c r="J41" s="1"/>
+      <c r="K41" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M40" s="1"/>
-      <c r="N40" s="9" t="s">
+      <c r="M41" s="1"/>
+      <c r="N41" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="9" t="s">
+      <c r="P41" s="1"/>
+      <c r="Q41" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S40" s="1"/>
-      <c r="T40" s="9" t="s">
+      <c r="S41" s="1"/>
+      <c r="T41" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J41" s="1"/>
-      <c r="K41" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M41" s="1"/>
-      <c r="N41" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S41" s="1"/>
-      <c r="T41" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="12">
-        <f>SUM(D10:D38)</f>
-        <v>82.5</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="12">
-        <f>SUM(G10:G38)</f>
-        <v>120</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" s="12">
-        <f>SUM(J10:J38)</f>
-        <v>10</v>
-      </c>
-      <c r="M42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N42" s="12">
-        <f>SUM(M10:M38)</f>
-        <v>85</v>
-      </c>
-      <c r="P42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q42" s="12">
-        <f>SUM(P10:P38)</f>
-        <v>-30</v>
-      </c>
-      <c r="S42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T42" s="12">
-        <f>SUM(S10:S38)</f>
-        <v>-267.5</v>
-      </c>
-      <c r="U42" s="1">
-        <f>SUM(E42,H42,K42,N42,Q42,T42)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D42" s="1"/>
+      <c r="E42" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J42" s="1"/>
+      <c r="K42" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M42" s="1"/>
+      <c r="N42" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S42" s="1"/>
+      <c r="T42" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+      <c r="D43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="12">
+        <f>SUM(D10:D39)</f>
+        <v>57.5</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="12">
+        <f>SUM(G10:G39)</f>
+        <v>170</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="12">
+        <f>SUM(J10:J39)</f>
+        <v>-5</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N43" s="12">
+        <f>SUM(M10:M39)</f>
+        <v>75</v>
+      </c>
+      <c r="P43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q43" s="12">
+        <f>SUM(P10:P39)</f>
+        <v>-10</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T43" s="12">
+        <f>SUM(S10:S39)</f>
+        <v>-287.5</v>
+      </c>
+      <c r="U43" s="1">
+        <f>SUM(E43,H43,K43,N43,Q43,T43)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
@@ -2587,6 +2636,13 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2598,7 +2654,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E42">
+  <conditionalFormatting sqref="E43">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2609,7 +2665,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K42">
+  <conditionalFormatting sqref="K43">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2620,7 +2676,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
+  <conditionalFormatting sqref="H43">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2631,7 +2687,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N42">
+  <conditionalFormatting sqref="N43">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2642,7 +2698,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T42">
+  <conditionalFormatting sqref="T43">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2653,7 +2709,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q42">
+  <conditionalFormatting sqref="Q43">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 21 KKR vs CSK.
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65DBA3E-A983-4A4D-B84F-54E80713B26F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2E613A-B1C5-144D-9248-A117D39C317D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="2240" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2200" yWindow="1960" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Points</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>SRH vs CSK</t>
+  </si>
+  <si>
+    <t>DC vs RR</t>
   </si>
 </sst>
 </file>
@@ -846,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U47"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2088,36 +2091,48 @@
       <c r="C30" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="3" t="str">
+      <c r="D30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="G30" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E30" s="4">
+        <v>80</v>
+      </c>
+      <c r="G30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H30" s="4"/>
-      <c r="J30" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K30" s="4"/>
-      <c r="M30" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K30" s="4">
+        <v>100</v>
+      </c>
+      <c r="M30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N30" s="4"/>
-      <c r="P30" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N30" s="4">
+        <v>40</v>
+      </c>
+      <c r="P30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q30" s="4"/>
-      <c r="S30" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>20</v>
+      </c>
+      <c r="S30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T30" s="4"/>
+        <v>-10</v>
+      </c>
+      <c r="T30" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -2448,9 +2463,15 @@
       <c r="T38" s="4"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="13"/>
+      <c r="A39" s="1">
+        <v>30</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="D39" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2485,143 +2506,171 @@
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="G40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H40" s="4"/>
-      <c r="J40" s="4"/>
+      <c r="J40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="M40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N40" s="4"/>
-      <c r="P40" s="4"/>
+      <c r="P40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q40" s="4"/>
-      <c r="S40" s="4"/>
+      <c r="S40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="6"/>
-      <c r="B41" s="1" t="s">
+      <c r="A41" s="1"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="9" t="s">
+      <c r="C42" s="10"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="9" t="s">
+      <c r="G42" s="1"/>
+      <c r="H42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J41" s="1"/>
-      <c r="K41" s="9" t="s">
+      <c r="J42" s="1"/>
+      <c r="K42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M41" s="1"/>
-      <c r="N41" s="9" t="s">
+      <c r="M42" s="1"/>
+      <c r="N42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="9" t="s">
+      <c r="P42" s="1"/>
+      <c r="Q42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S41" s="1"/>
-      <c r="T41" s="9" t="s">
+      <c r="S42" s="1"/>
+      <c r="T42" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J42" s="1"/>
-      <c r="K42" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M42" s="1"/>
-      <c r="N42" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S42" s="1"/>
-      <c r="T42" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
-      <c r="D43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="12">
-        <f>SUM(D10:D39)</f>
-        <v>57.5</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="12">
-        <f>SUM(G10:G39)</f>
-        <v>170</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K43" s="12">
-        <f>SUM(J10:J39)</f>
-        <v>-5</v>
-      </c>
-      <c r="M43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N43" s="12">
-        <f>SUM(M10:M39)</f>
-        <v>75</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q43" s="12">
-        <f>SUM(P10:P39)</f>
-        <v>-10</v>
-      </c>
-      <c r="S43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T43" s="12">
-        <f>SUM(S10:S39)</f>
-        <v>-287.5</v>
-      </c>
-      <c r="U43" s="1">
-        <f>SUM(E43,H43,K43,N43,Q43,T43)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D43" s="1"/>
+      <c r="E43" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J43" s="1"/>
+      <c r="K43" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M43" s="1"/>
+      <c r="N43" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S43" s="1"/>
+      <c r="T43" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="D44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="12">
+        <f>SUM(D10:D40)</f>
+        <v>77.5</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="12">
+        <f>SUM(G10:G40)</f>
+        <v>145</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="12">
+        <f>SUM(J10:J40)</f>
+        <v>45</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N44" s="12">
+        <f>SUM(M10:M40)</f>
+        <v>60</v>
+      </c>
+      <c r="P44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q44" s="12">
+        <f>SUM(P10:P40)</f>
+        <v>-30</v>
+      </c>
+      <c r="S44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T44" s="12">
+        <f>SUM(S10:S40)</f>
+        <v>-297.5</v>
+      </c>
+      <c r="U44" s="1">
+        <f>SUM(E44,H44,K44,N44,Q44,T44)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
@@ -2643,6 +2692,13 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2654,7 +2710,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E43">
+  <conditionalFormatting sqref="E44">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2665,7 +2721,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
+  <conditionalFormatting sqref="K44">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2676,7 +2732,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="H44">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2687,7 +2743,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N43">
+  <conditionalFormatting sqref="N44">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2698,7 +2754,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T43">
+  <conditionalFormatting sqref="T44">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2709,7 +2765,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q43">
+  <conditionalFormatting sqref="Q44">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 22 SRH vs KXI
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2E613A-B1C5-144D-9248-A117D39C317D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD73B108-BEA7-6944-BA11-BA3D80778CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1960" windowWidth="32600" windowHeight="19000" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2480" yWindow="560" windowWidth="32980" windowHeight="19960" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Points</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>DC vs RR</t>
+  </si>
+  <si>
+    <t>RCB vs KXI</t>
   </si>
 </sst>
 </file>
@@ -849,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U48"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="V37" sqref="V37"/>
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2144,36 +2147,48 @@
       <c r="C31" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="G31" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E31" s="4">
+        <v>60</v>
+      </c>
+      <c r="G31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H31" s="4"/>
-      <c r="J31" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H31" s="4">
+        <v>40</v>
+      </c>
+      <c r="J31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K31" s="4"/>
-      <c r="M31" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K31" s="4">
+        <v>20</v>
+      </c>
+      <c r="M31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N31" s="4"/>
-      <c r="P31" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N31" s="4">
+        <v>100</v>
+      </c>
+      <c r="P31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q31" s="4"/>
-      <c r="S31" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>80</v>
+      </c>
+      <c r="S31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T31" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T31" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -2504,9 +2519,15 @@
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="13"/>
+      <c r="A40" s="1">
+        <v>31</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="D40" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2541,143 +2562,171 @@
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="G41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H41" s="4"/>
-      <c r="J41" s="4"/>
+      <c r="J41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K41" s="4"/>
-      <c r="M41" s="4"/>
+      <c r="M41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N41" s="4"/>
-      <c r="P41" s="4"/>
+      <c r="P41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q41" s="4"/>
-      <c r="S41" s="4"/>
+      <c r="S41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T41" s="4"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
-      <c r="B42" s="1" t="s">
+      <c r="A42" s="1"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A43" s="6"/>
+      <c r="B43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="9" t="s">
+      <c r="C43" s="10"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="9" t="s">
+      <c r="G43" s="1"/>
+      <c r="H43" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J42" s="1"/>
-      <c r="K42" s="9" t="s">
+      <c r="J43" s="1"/>
+      <c r="K43" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M42" s="1"/>
-      <c r="N42" s="9" t="s">
+      <c r="M43" s="1"/>
+      <c r="N43" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="9" t="s">
+      <c r="P43" s="1"/>
+      <c r="Q43" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S42" s="1"/>
-      <c r="T42" s="9" t="s">
+      <c r="S43" s="1"/>
+      <c r="T43" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J43" s="1"/>
-      <c r="K43" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M43" s="1"/>
-      <c r="N43" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S43" s="1"/>
-      <c r="T43" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="12">
-        <f>SUM(D10:D40)</f>
-        <v>77.5</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="12">
-        <f>SUM(G10:G40)</f>
-        <v>145</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" s="12">
-        <f>SUM(J10:J40)</f>
-        <v>45</v>
-      </c>
-      <c r="M44" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N44" s="12">
-        <f>SUM(M10:M40)</f>
-        <v>60</v>
-      </c>
-      <c r="P44" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q44" s="12">
-        <f>SUM(P10:P40)</f>
-        <v>-30</v>
-      </c>
-      <c r="S44" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T44" s="12">
-        <f>SUM(S10:S40)</f>
-        <v>-297.5</v>
-      </c>
-      <c r="U44" s="1">
-        <f>SUM(E44,H44,K44,N44,Q44,T44)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D44" s="1"/>
+      <c r="E44" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J44" s="1"/>
+      <c r="K44" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M44" s="1"/>
+      <c r="N44" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S44" s="1"/>
+      <c r="T44" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="D45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="12">
+        <f>SUM(D10:D41)</f>
+        <v>67.5</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="12">
+        <f>SUM(G10:G41)</f>
+        <v>130</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45" s="12">
+        <f>SUM(J10:J41)</f>
+        <v>25</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N45" s="12">
+        <f>SUM(M10:M41)</f>
+        <v>110</v>
+      </c>
+      <c r="P45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q45" s="12">
+        <f>SUM(P10:P41)</f>
+        <v>-10</v>
+      </c>
+      <c r="S45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T45" s="12">
+        <f>SUM(S10:S41)</f>
+        <v>-322.5</v>
+      </c>
+      <c r="U45" s="1">
+        <f>SUM(E45,H45,K45,N45,Q45,T45)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
@@ -2699,6 +2748,13 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2710,7 +2766,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E44">
+  <conditionalFormatting sqref="E45">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2721,7 +2777,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K44">
+  <conditionalFormatting sqref="K45">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2732,7 +2788,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44">
+  <conditionalFormatting sqref="H45">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2743,7 +2799,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N44">
+  <conditionalFormatting sqref="N45">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2754,7 +2810,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T44">
+  <conditionalFormatting sqref="T45">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2765,7 +2821,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q44">
+  <conditionalFormatting sqref="Q45">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 23 RR vs DC
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD73B108-BEA7-6944-BA11-BA3D80778CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8B7449-A045-2643-A233-CAD0C33A9706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2480" yWindow="560" windowWidth="32980" windowHeight="19960" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Points</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>RCB vs KXI</t>
+  </si>
+  <si>
+    <t>MI vs KKR</t>
   </si>
 </sst>
 </file>
@@ -852,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U49"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+      <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2200,36 +2203,48 @@
       <c r="C32" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="3" t="str">
+      <c r="D32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="G32" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E32" s="4">
+        <v>80</v>
+      </c>
+      <c r="G32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="J32" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H32" s="4">
+        <v>40</v>
+      </c>
+      <c r="J32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K32" s="4"/>
-      <c r="M32" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K32" s="4">
+        <v>60</v>
+      </c>
+      <c r="M32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N32" s="4"/>
-      <c r="P32" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
+      <c r="P32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q32" s="4"/>
-      <c r="S32" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>20</v>
+      </c>
+      <c r="S32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T32" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="T32" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -2560,9 +2575,15 @@
       <c r="T40" s="4"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="13"/>
+      <c r="A41" s="1">
+        <v>32</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="D41" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2597,143 +2618,171 @@
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="G42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H42" s="4"/>
-      <c r="J42" s="4"/>
+      <c r="J42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K42" s="4"/>
-      <c r="M42" s="4"/>
+      <c r="M42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N42" s="4"/>
-      <c r="P42" s="4"/>
+      <c r="P42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q42" s="4"/>
-      <c r="S42" s="4"/>
+      <c r="S42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T42" s="4"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="6"/>
-      <c r="B43" s="1" t="s">
+      <c r="A43" s="1"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="9" t="s">
+      <c r="C44" s="10"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="9" t="s">
+      <c r="G44" s="1"/>
+      <c r="H44" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J43" s="1"/>
-      <c r="K43" s="9" t="s">
+      <c r="J44" s="1"/>
+      <c r="K44" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M43" s="1"/>
-      <c r="N43" s="9" t="s">
+      <c r="M44" s="1"/>
+      <c r="N44" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="9" t="s">
+      <c r="P44" s="1"/>
+      <c r="Q44" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S43" s="1"/>
-      <c r="T43" s="9" t="s">
+      <c r="S44" s="1"/>
+      <c r="T44" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J44" s="1"/>
-      <c r="K44" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M44" s="1"/>
-      <c r="N44" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S44" s="1"/>
-      <c r="T44" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" s="12">
-        <f>SUM(D10:D41)</f>
-        <v>67.5</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" s="12">
-        <f>SUM(G10:G41)</f>
-        <v>130</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K45" s="12">
-        <f>SUM(J10:J41)</f>
-        <v>25</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N45" s="12">
-        <f>SUM(M10:M41)</f>
-        <v>110</v>
-      </c>
-      <c r="P45" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q45" s="12">
-        <f>SUM(P10:P41)</f>
-        <v>-10</v>
-      </c>
-      <c r="S45" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T45" s="12">
-        <f>SUM(S10:S41)</f>
-        <v>-322.5</v>
-      </c>
-      <c r="U45" s="1">
-        <f>SUM(E45,H45,K45,N45,Q45,T45)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D45" s="1"/>
+      <c r="E45" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J45" s="1"/>
+      <c r="K45" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S45" s="1"/>
+      <c r="T45" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
+      <c r="D46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="12">
+        <f>SUM(D10:D42)</f>
+        <v>87.5</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="12">
+        <f>SUM(G10:G42)</f>
+        <v>115</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K46" s="12">
+        <f>SUM(J10:J42)</f>
+        <v>15</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N46" s="12">
+        <f>SUM(M10:M42)</f>
+        <v>85</v>
+      </c>
+      <c r="P46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q46" s="12">
+        <f>SUM(P10:P42)</f>
+        <v>-30</v>
+      </c>
+      <c r="S46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T46" s="12">
+        <f>SUM(S10:S42)</f>
+        <v>-272.5</v>
+      </c>
+      <c r="U46" s="1">
+        <f>SUM(E46,H46,K46,N46,Q46,T46)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
@@ -2755,6 +2804,13 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2766,7 +2822,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E45">
+  <conditionalFormatting sqref="E46">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2777,7 +2833,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K45">
+  <conditionalFormatting sqref="K46">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2788,7 +2844,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
+  <conditionalFormatting sqref="H46">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2799,7 +2855,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N45">
+  <conditionalFormatting sqref="N46">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2810,7 +2866,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T45">
+  <conditionalFormatting sqref="T46">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2821,7 +2877,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q45">
+  <conditionalFormatting sqref="Q46">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 24 KXI vs KKR and Contest 25 CSK vs RCB
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8B7449-A045-2643-A233-CAD0C33A9706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1FFBE2-2C1A-BF4F-9543-3F6CDC2E2DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="560" windowWidth="32980" windowHeight="19960" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2220" yWindow="560" windowWidth="32980" windowHeight="19960" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>Points</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>MI vs KKR</t>
+  </si>
+  <si>
+    <t>RR vs RCB</t>
+  </si>
+  <si>
+    <t>DC vs CSK</t>
   </si>
 </sst>
 </file>
@@ -855,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U50"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U46" sqref="U46"/>
+      <selection activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2256,36 +2262,46 @@
       <c r="C33" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="G33" s="3" t="str">
+      <c r="D33" s="3">
+        <v>-17.5</v>
+      </c>
+      <c r="E33" s="4">
+        <v>40</v>
+      </c>
+      <c r="G33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H33" s="4"/>
-      <c r="J33" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K33" s="4"/>
-      <c r="M33" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K33" s="4">
+        <v>60</v>
+      </c>
+      <c r="M33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N33" s="4"/>
-      <c r="P33" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N33" s="4">
+        <v>80</v>
+      </c>
+      <c r="P33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q33" s="4"/>
-      <c r="S33" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T33" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>100</v>
+      </c>
+      <c r="S33" s="3">
+        <v>-17.5</v>
+      </c>
+      <c r="T33" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -2297,36 +2313,48 @@
       <c r="C34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E34" s="4"/>
-      <c r="G34" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E34" s="4">
+        <v>60</v>
+      </c>
+      <c r="G34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H34" s="4"/>
-      <c r="J34" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H34" s="4">
+        <v>40</v>
+      </c>
+      <c r="J34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K34" s="4"/>
-      <c r="M34" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K34" s="4">
+        <v>100</v>
+      </c>
+      <c r="M34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N34" s="4"/>
-      <c r="P34" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N34" s="4">
+        <v>80</v>
+      </c>
+      <c r="P34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q34" s="4"/>
-      <c r="S34" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>20</v>
+      </c>
+      <c r="S34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T34" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T34" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -2616,9 +2644,15 @@
       <c r="T41" s="4"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="13"/>
+      <c r="A42" s="1">
+        <v>33</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="D42" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2651,152 +2685,214 @@
       <c r="T42" s="4"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="A43" s="1">
+        <v>34</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="J43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K43" s="4"/>
-      <c r="M43" s="4"/>
+      <c r="M43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N43" s="4"/>
-      <c r="P43" s="4"/>
+      <c r="P43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q43" s="4"/>
-      <c r="S43" s="4"/>
+      <c r="S43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T43" s="4"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
-      <c r="B44" s="1" t="s">
+      <c r="A44" s="1"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="G44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H44" s="4"/>
+      <c r="J44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K44" s="4"/>
+      <c r="M44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N44" s="4"/>
+      <c r="P44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q44" s="4"/>
+      <c r="S44" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T44" s="4"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A46" s="6"/>
+      <c r="B46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="9" t="s">
+      <c r="C46" s="10"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="9" t="s">
+      <c r="G46" s="1"/>
+      <c r="H46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="1"/>
-      <c r="K44" s="9" t="s">
+      <c r="J46" s="1"/>
+      <c r="K46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M44" s="1"/>
-      <c r="N44" s="9" t="s">
+      <c r="M46" s="1"/>
+      <c r="N46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="9" t="s">
+      <c r="P46" s="1"/>
+      <c r="Q46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S44" s="1"/>
-      <c r="T44" s="9" t="s">
+      <c r="S46" s="1"/>
+      <c r="T46" s="9" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J45" s="1"/>
-      <c r="K45" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M45" s="1"/>
-      <c r="N45" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S45" s="1"/>
-      <c r="T45" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" s="12">
-        <f>SUM(D10:D42)</f>
-        <v>87.5</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="12">
-        <f>SUM(G10:G42)</f>
-        <v>115</v>
-      </c>
-      <c r="J46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K46" s="12">
-        <f>SUM(J10:J42)</f>
-        <v>15</v>
-      </c>
-      <c r="M46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N46" s="12">
-        <f>SUM(M10:M42)</f>
-        <v>85</v>
-      </c>
-      <c r="P46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q46" s="12">
-        <f>SUM(P10:P42)</f>
-        <v>-30</v>
-      </c>
-      <c r="S46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T46" s="12">
-        <f>SUM(S10:S42)</f>
-        <v>-272.5</v>
-      </c>
-      <c r="U46" s="1">
-        <f>SUM(E46,H46,K46,N46,Q46,T46)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D47" s="1"/>
+      <c r="E47" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J47" s="1"/>
+      <c r="K47" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M47" s="1"/>
+      <c r="N47" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S47" s="1"/>
+      <c r="T47" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+      <c r="D48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="12">
+        <f>SUM(D10:D44)</f>
+        <v>60</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="12">
+        <f>SUM(G10:G44)</f>
+        <v>75</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" s="12">
+        <f>SUM(J10:J44)</f>
+        <v>55</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N48" s="12">
+        <f>SUM(M10:M44)</f>
+        <v>125</v>
+      </c>
+      <c r="P48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q48" s="12">
+        <f>SUM(P10:P44)</f>
+        <v>0</v>
+      </c>
+      <c r="S48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T48" s="12">
+        <f>SUM(S10:S44)</f>
+        <v>-315</v>
+      </c>
+      <c r="U48" s="1">
+        <f>SUM(E48,H48,K48,N48,Q48,T48)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
@@ -2811,6 +2907,20 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2822,7 +2932,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E48">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2833,7 +2943,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
+  <conditionalFormatting sqref="K48">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2844,7 +2954,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46">
+  <conditionalFormatting sqref="H48">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2855,7 +2965,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46">
+  <conditionalFormatting sqref="N48">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2866,7 +2976,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T46">
+  <conditionalFormatting sqref="T48">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2877,7 +2987,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q46">
+  <conditionalFormatting sqref="Q48">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Results: Contest 26 SRH vs RR & Contest 27 MI vs DC
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1FFBE2-2C1A-BF4F-9543-3F6CDC2E2DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14486646-39D2-C341-A001-EDD51F6F49BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="560" windowWidth="32980" windowHeight="19960" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="1540" yWindow="900" windowWidth="32980" windowHeight="19960" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
   <si>
     <t>Points</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>DC vs CSK</t>
+  </si>
+  <si>
+    <t>SRH vs KKR</t>
+  </si>
+  <si>
+    <t>MI vs KXI</t>
   </si>
 </sst>
 </file>
@@ -861,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U48" sqref="U48"/>
+      <selection activeCell="U50" sqref="U50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2252,7 +2258,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -2303,7 +2309,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>25</v>
       </c>
@@ -2356,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>26</v>
       </c>
@@ -2366,38 +2372,50 @@
       <c r="C35" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="G35" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E35" s="4">
+        <v>60</v>
+      </c>
+      <c r="G35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="J35" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H35" s="4">
+        <v>80</v>
+      </c>
+      <c r="J35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K35" s="4"/>
-      <c r="M35" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K35" s="4">
+        <v>40</v>
+      </c>
+      <c r="M35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N35" s="4"/>
-      <c r="P35" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N35" s="4">
+        <v>100</v>
+      </c>
+      <c r="P35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q35" s="4"/>
-      <c r="S35" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>20</v>
+      </c>
+      <c r="S35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T35" s="4"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-25</v>
+      </c>
+      <c r="T35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>27</v>
       </c>
@@ -2407,38 +2425,50 @@
       <c r="C36" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="G36" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E36" s="4">
+        <v>80</v>
+      </c>
+      <c r="G36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H36" s="4"/>
-      <c r="J36" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H36" s="4">
+        <v>60</v>
+      </c>
+      <c r="J36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K36" s="4"/>
-      <c r="M36" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K36" s="4">
+        <v>100</v>
+      </c>
+      <c r="M36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N36" s="4"/>
-      <c r="P36" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N36" s="4">
+        <v>20</v>
+      </c>
+      <c r="P36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q36" s="4"/>
-      <c r="S36" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>40</v>
+      </c>
+      <c r="S36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T36" s="4"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-25</v>
+      </c>
+      <c r="T36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>28</v>
       </c>
@@ -2479,7 +2509,7 @@
       </c>
       <c r="T37" s="4"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>29</v>
       </c>
@@ -2520,7 +2550,7 @@
       </c>
       <c r="T38" s="4"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>30</v>
       </c>
@@ -2561,7 +2591,7 @@
       </c>
       <c r="T39" s="4"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>31</v>
       </c>
@@ -2602,7 +2632,7 @@
       </c>
       <c r="T40" s="4"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>32</v>
       </c>
@@ -2643,7 +2673,7 @@
       </c>
       <c r="T41" s="4"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>33</v>
       </c>
@@ -2684,7 +2714,7 @@
       </c>
       <c r="T42" s="4"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>34</v>
       </c>
@@ -2725,10 +2755,16 @@
       </c>
       <c r="T43" s="4"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="13"/>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>35</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>55</v>
+      </c>
       <c r="D44" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2760,167 +2796,243 @@
       </c>
       <c r="T44" s="4"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>36</v>
+      </c>
+      <c r="B45" s="4">
+        <v>1</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="G45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H45" s="4"/>
-      <c r="J45" s="4"/>
+      <c r="J45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K45" s="4"/>
-      <c r="M45" s="4"/>
+      <c r="M45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N45" s="4"/>
-      <c r="P45" s="4"/>
+      <c r="P45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q45" s="4"/>
-      <c r="S45" s="4"/>
+      <c r="S45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T45" s="4"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A46" s="6"/>
-      <c r="B46" s="1" t="s">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="G46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H46" s="4"/>
+      <c r="J46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K46" s="4"/>
+      <c r="M46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N46" s="4"/>
+      <c r="P46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q46" s="4"/>
+      <c r="S46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T46" s="4"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A48" s="6"/>
+      <c r="B48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="9" t="s">
+      <c r="C48" s="10"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="9" t="s">
+      <c r="G48" s="1"/>
+      <c r="H48" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J46" s="1"/>
-      <c r="K46" s="9" t="s">
+      <c r="J48" s="1"/>
+      <c r="K48" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="1"/>
-      <c r="N46" s="9" t="s">
+      <c r="M48" s="1"/>
+      <c r="N48" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="9" t="s">
+      <c r="P48" s="1"/>
+      <c r="Q48" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S46" s="1"/>
-      <c r="T46" s="9" t="s">
+      <c r="S48" s="1"/>
+      <c r="T48" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J47" s="1"/>
-      <c r="K47" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M47" s="1"/>
-      <c r="N47" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S47" s="1"/>
-      <c r="T47" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="12">
-        <f>SUM(D10:D44)</f>
-        <v>60</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="12">
-        <f>SUM(G10:G44)</f>
-        <v>75</v>
-      </c>
-      <c r="J48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K48" s="12">
-        <f>SUM(J10:J44)</f>
-        <v>55</v>
-      </c>
-      <c r="M48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N48" s="12">
-        <f>SUM(M10:M44)</f>
-        <v>125</v>
-      </c>
-      <c r="P48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q48" s="12">
-        <f>SUM(P10:P44)</f>
-        <v>0</v>
-      </c>
-      <c r="S48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T48" s="12">
-        <f>SUM(S10:S44)</f>
-        <v>-315</v>
-      </c>
-      <c r="U48" s="1">
-        <f>SUM(E48,H48,K48,N48,Q48,T48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D49" s="1"/>
+      <c r="E49" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J49" s="1"/>
+      <c r="K49" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M49" s="1"/>
+      <c r="N49" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S49" s="1"/>
+      <c r="T49" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="12">
+        <f>SUM(D10:D46)</f>
+        <v>70</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="12">
+        <f>SUM(G10:G46)</f>
+        <v>85</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K50" s="12">
+        <f>SUM(J10:J46)</f>
+        <v>90</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N50" s="12">
+        <f>SUM(M10:M46)</f>
+        <v>155</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q50" s="12">
+        <f>SUM(P10:P46)</f>
+        <v>-35</v>
+      </c>
+      <c r="S50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T50" s="12">
+        <f>SUM(S10:S46)</f>
+        <v>-365</v>
+      </c>
+      <c r="U50" s="1">
+        <f>SUM(E50,H50,K50,N50,Q50,T50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2932,7 +3044,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E48">
+  <conditionalFormatting sqref="E50">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2943,7 +3055,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K48">
+  <conditionalFormatting sqref="K50">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2954,7 +3066,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
+  <conditionalFormatting sqref="H50">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2965,7 +3077,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N48">
+  <conditionalFormatting sqref="N50">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2976,7 +3088,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T48">
+  <conditionalFormatting sqref="T50">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2987,7 +3099,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q48">
+  <conditionalFormatting sqref="Q50">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 28 RCB vs KKR - RCB won.
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14486646-39D2-C341-A001-EDD51F6F49BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D7187A-3D50-6F4E-8D6D-AFD3A51F287B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="900" windowWidth="32980" windowHeight="19960" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Points</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>MI vs KXI</t>
+  </si>
+  <si>
+    <t>CSK vs RR</t>
   </si>
 </sst>
 </file>
@@ -867,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U54"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U50" sqref="U50"/>
+      <selection activeCell="U51" sqref="U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2478,36 +2481,48 @@
       <c r="C37" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="G37" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E37" s="4">
+        <v>80</v>
+      </c>
+      <c r="G37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="J37" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K37" s="4"/>
-      <c r="M37" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K37" s="4">
+        <v>60</v>
+      </c>
+      <c r="M37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N37" s="4"/>
-      <c r="P37" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N37" s="4">
+        <v>100</v>
+      </c>
+      <c r="P37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q37" s="4"/>
-      <c r="S37" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>40</v>
+      </c>
+      <c r="S37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T37" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T37" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -2838,9 +2853,15 @@
       <c r="T45" s="4"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="13"/>
+      <c r="A46" s="1">
+        <v>37</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="D46" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2875,143 +2896,171 @@
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="G47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H47" s="4"/>
-      <c r="J47" s="4"/>
+      <c r="J47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K47" s="4"/>
-      <c r="M47" s="4"/>
+      <c r="M47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N47" s="4"/>
-      <c r="P47" s="4"/>
+      <c r="P47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q47" s="4"/>
-      <c r="S47" s="4"/>
+      <c r="S47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T47" s="4"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A48" s="6"/>
-      <c r="B48" s="1" t="s">
+      <c r="A48" s="1"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A49" s="6"/>
+      <c r="B49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="9" t="s">
+      <c r="C49" s="10"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="9" t="s">
+      <c r="G49" s="1"/>
+      <c r="H49" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J48" s="1"/>
-      <c r="K48" s="9" t="s">
+      <c r="J49" s="1"/>
+      <c r="K49" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M48" s="1"/>
-      <c r="N48" s="9" t="s">
+      <c r="M49" s="1"/>
+      <c r="N49" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="9" t="s">
+      <c r="P49" s="1"/>
+      <c r="Q49" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S48" s="1"/>
-      <c r="T48" s="9" t="s">
+      <c r="S49" s="1"/>
+      <c r="T49" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M49" s="1"/>
-      <c r="N49" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S49" s="1"/>
-      <c r="T49" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" s="12">
-        <f>SUM(D10:D46)</f>
-        <v>70</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="12">
-        <f>SUM(G10:G46)</f>
-        <v>85</v>
-      </c>
-      <c r="J50" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K50" s="12">
-        <f>SUM(J10:J46)</f>
-        <v>90</v>
-      </c>
-      <c r="M50" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N50" s="12">
-        <f>SUM(M10:M46)</f>
-        <v>155</v>
-      </c>
-      <c r="P50" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q50" s="12">
-        <f>SUM(P10:P46)</f>
-        <v>-35</v>
-      </c>
-      <c r="S50" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T50" s="12">
-        <f>SUM(S10:S46)</f>
-        <v>-365</v>
-      </c>
-      <c r="U50" s="1">
-        <f>SUM(E50,H50,K50,N50,Q50,T50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D50" s="1"/>
+      <c r="E50" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J50" s="1"/>
+      <c r="K50" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M50" s="1"/>
+      <c r="N50" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S50" s="1"/>
+      <c r="T50" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="D51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="12">
+        <f>SUM(D10:D47)</f>
+        <v>90</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="12">
+        <f>SUM(G10:G47)</f>
+        <v>60</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K51" s="12">
+        <f>SUM(J10:J47)</f>
+        <v>80</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N51" s="12">
+        <f>SUM(M10:M47)</f>
+        <v>205</v>
+      </c>
+      <c r="P51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q51" s="12">
+        <f>SUM(P10:P47)</f>
+        <v>-50</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T51" s="12">
+        <f>SUM(S10:S47)</f>
+        <v>-385</v>
+      </c>
+      <c r="U51" s="1">
+        <f>SUM(E51,H51,K51,N51,Q51,T51)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
@@ -3033,6 +3082,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3044,7 +3100,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E50">
+  <conditionalFormatting sqref="E51">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3055,7 +3111,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K50">
+  <conditionalFormatting sqref="K51">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3066,7 +3122,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
+  <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3077,7 +3133,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N51">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3088,7 +3144,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T50">
+  <conditionalFormatting sqref="T51">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3099,7 +3155,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q50">
+  <conditionalFormatting sqref="Q51">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 29 SRH vs CSK
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D7187A-3D50-6F4E-8D6D-AFD3A51F287B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFDEC4B-1470-FC47-BF78-5B56626F8147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="900" windowWidth="32980" windowHeight="19960" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2200" yWindow="460" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>Points</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>CSK vs RR</t>
+  </si>
+  <si>
+    <t>KXI vs DC</t>
   </si>
 </sst>
 </file>
@@ -870,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U55"/>
+  <dimension ref="A1:U56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U51" sqref="U51"/>
+      <selection activeCell="U52" sqref="U52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2534,36 +2537,48 @@
       <c r="C38" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="D38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="G38" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E38" s="4">
+        <v>20</v>
+      </c>
+      <c r="G38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="J38" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H38" s="4">
+        <v>40</v>
+      </c>
+      <c r="J38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K38" s="4"/>
-      <c r="M38" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K38" s="4">
+        <v>0</v>
+      </c>
+      <c r="M38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N38" s="4"/>
-      <c r="P38" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N38" s="4">
+        <v>60</v>
+      </c>
+      <c r="P38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q38" s="4"/>
-      <c r="S38" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>80</v>
+      </c>
+      <c r="S38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T38" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="T38" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -2894,9 +2909,15 @@
       <c r="T46" s="4"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="13"/>
+      <c r="A47" s="1">
+        <v>38</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="D47" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2931,143 +2952,171 @@
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="G48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H48" s="4"/>
-      <c r="J48" s="4"/>
+      <c r="J48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K48" s="4"/>
-      <c r="M48" s="4"/>
+      <c r="M48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N48" s="4"/>
-      <c r="P48" s="4"/>
+      <c r="P48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q48" s="4"/>
-      <c r="S48" s="4"/>
+      <c r="S48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T48" s="4"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A49" s="6"/>
-      <c r="B49" s="1" t="s">
+      <c r="A49" s="1"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A50" s="6"/>
+      <c r="B50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="9" t="s">
+      <c r="C50" s="10"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="9" t="s">
+      <c r="G50" s="1"/>
+      <c r="H50" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J49" s="1"/>
-      <c r="K49" s="9" t="s">
+      <c r="J50" s="1"/>
+      <c r="K50" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M49" s="1"/>
-      <c r="N49" s="9" t="s">
+      <c r="M50" s="1"/>
+      <c r="N50" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="9" t="s">
+      <c r="P50" s="1"/>
+      <c r="Q50" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S49" s="1"/>
-      <c r="T49" s="9" t="s">
+      <c r="S50" s="1"/>
+      <c r="T50" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J50" s="1"/>
-      <c r="K50" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M50" s="1"/>
-      <c r="N50" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S50" s="1"/>
-      <c r="T50" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
-      <c r="D51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="12">
-        <f>SUM(D10:D47)</f>
-        <v>90</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="12">
-        <f>SUM(G10:G47)</f>
-        <v>60</v>
-      </c>
-      <c r="J51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K51" s="12">
-        <f>SUM(J10:J47)</f>
-        <v>80</v>
-      </c>
-      <c r="M51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N51" s="12">
-        <f>SUM(M10:M47)</f>
-        <v>205</v>
-      </c>
-      <c r="P51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q51" s="12">
-        <f>SUM(P10:P47)</f>
-        <v>-50</v>
-      </c>
-      <c r="S51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T51" s="12">
-        <f>SUM(S10:S47)</f>
-        <v>-385</v>
-      </c>
-      <c r="U51" s="1">
-        <f>SUM(E51,H51,K51,N51,Q51,T51)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D51" s="1"/>
+      <c r="E51" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J51" s="1"/>
+      <c r="K51" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S51" s="1"/>
+      <c r="T51" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
+      <c r="D52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="12">
+        <f>SUM(D10:D48)</f>
+        <v>70</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="12">
+        <f>SUM(G10:G48)</f>
+        <v>45</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K52" s="12">
+        <f>SUM(J10:J48)</f>
+        <v>55</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N52" s="12">
+        <f>SUM(M10:M48)</f>
+        <v>195</v>
+      </c>
+      <c r="P52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q52" s="12">
+        <f>SUM(P10:P48)</f>
+        <v>-30</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T52" s="12">
+        <f>SUM(S10:S48)</f>
+        <v>-335</v>
+      </c>
+      <c r="U52" s="1">
+        <f>SUM(E52,H52,K52,N52,Q52,T52)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
@@ -3089,6 +3138,13 @@
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3100,7 +3156,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E52">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3111,7 +3167,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K51">
+  <conditionalFormatting sqref="K52">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3122,7 +3178,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
+  <conditionalFormatting sqref="H52">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3133,7 +3189,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N51">
+  <conditionalFormatting sqref="N52">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3144,7 +3200,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T51">
+  <conditionalFormatting sqref="T52">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3155,7 +3211,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q51">
+  <conditionalFormatting sqref="Q52">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Results: Contest 33 RR vs RCB & Contest 34 DC vs CSK
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFDEC4B-1470-FC47-BF78-5B56626F8147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA20609-DFEA-AC40-BD88-1BF355909CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="460" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>Points</t>
   </si>
@@ -207,6 +207,21 @@
   </si>
   <si>
     <t>KXI vs DC</t>
+  </si>
+  <si>
+    <t>KKR vs RCB</t>
+  </si>
+  <si>
+    <t>RR vs SRH</t>
+  </si>
+  <si>
+    <t>CSK vs MI</t>
+  </si>
+  <si>
+    <t>KKR vs DC</t>
+  </si>
+  <si>
+    <t>KXI vs SRH</t>
   </si>
 </sst>
 </file>
@@ -873,10 +888,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U56"/>
+  <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U52" sqref="U52"/>
+      <pane ySplit="8" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U57" sqref="U57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2590,36 +2606,48 @@
       <c r="C39" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="3" t="str">
+      <c r="D39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E39" s="4"/>
-      <c r="G39" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E39" s="4">
+        <v>80</v>
+      </c>
+      <c r="G39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H39" s="4"/>
-      <c r="J39" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H39" s="4">
+        <v>40</v>
+      </c>
+      <c r="J39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K39" s="4"/>
-      <c r="M39" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K39" s="4">
+        <v>0</v>
+      </c>
+      <c r="M39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N39" s="4"/>
-      <c r="P39" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N39" s="4">
+        <v>100</v>
+      </c>
+      <c r="P39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q39" s="4"/>
-      <c r="S39" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>60</v>
+      </c>
+      <c r="S39" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T39" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T39" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -2631,36 +2659,48 @@
       <c r="C40" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="3" t="str">
+      <c r="D40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="G40" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E40" s="4">
+        <v>80</v>
+      </c>
+      <c r="G40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H40" s="4"/>
-      <c r="J40" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H40" s="4">
+        <v>60</v>
+      </c>
+      <c r="J40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K40" s="4"/>
-      <c r="M40" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K40" s="4">
+        <v>100</v>
+      </c>
+      <c r="M40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N40" s="4"/>
-      <c r="P40" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N40" s="4">
+        <v>40</v>
+      </c>
+      <c r="P40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q40" s="4"/>
-      <c r="S40" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>20</v>
+      </c>
+      <c r="S40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T40" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T40" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -2672,36 +2712,48 @@
       <c r="C41" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="3" t="str">
+      <c r="D41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="G41" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E41" s="4">
+        <v>40</v>
+      </c>
+      <c r="G41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H41" s="4"/>
-      <c r="J41" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H41" s="4">
+        <v>80</v>
+      </c>
+      <c r="J41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K41" s="4"/>
-      <c r="M41" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K41" s="4">
+        <v>100</v>
+      </c>
+      <c r="M41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N41" s="4"/>
-      <c r="P41" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N41" s="4">
+        <v>60</v>
+      </c>
+      <c r="P41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q41" s="4"/>
-      <c r="S41" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>20</v>
+      </c>
+      <c r="S41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T41" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T41" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -2713,36 +2765,48 @@
       <c r="C42" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="3" t="str">
+      <c r="D42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="G42" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E42" s="4">
+        <v>80</v>
+      </c>
+      <c r="G42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="J42" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H42" s="4">
+        <v>60</v>
+      </c>
+      <c r="J42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K42" s="4"/>
-      <c r="M42" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K42" s="4">
+        <v>20</v>
+      </c>
+      <c r="M42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N42" s="4"/>
-      <c r="P42" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N42" s="4">
+        <v>0</v>
+      </c>
+      <c r="P42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q42" s="4"/>
-      <c r="S42" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q42" s="4">
+        <v>40</v>
+      </c>
+      <c r="S42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T42" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="T42" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -2754,36 +2818,48 @@
       <c r="C43" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="3" t="str">
+      <c r="D43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="G43" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E43" s="4">
+        <v>20</v>
+      </c>
+      <c r="G43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H43" s="4"/>
-      <c r="J43" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H43" s="4">
+        <v>80</v>
+      </c>
+      <c r="J43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K43" s="4"/>
-      <c r="M43" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K43" s="4">
+        <v>100</v>
+      </c>
+      <c r="M43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N43" s="4"/>
-      <c r="P43" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N43" s="4">
+        <v>0</v>
+      </c>
+      <c r="P43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q43" s="4"/>
-      <c r="S43" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>60</v>
+      </c>
+      <c r="S43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T43" s="4"/>
+        <v>-15</v>
+      </c>
+      <c r="T43" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -2950,9 +3026,15 @@
       <c r="T47" s="4"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="13"/>
+      <c r="A48" s="1">
+        <v>39</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="D48" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
         <v/>
@@ -2985,166 +3067,365 @@
       <c r="T48" s="4"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
+      <c r="A49" s="1">
+        <v>40</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="G49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H49" s="4"/>
-      <c r="J49" s="4"/>
+      <c r="J49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K49" s="4"/>
-      <c r="M49" s="4"/>
+      <c r="M49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N49" s="4"/>
-      <c r="P49" s="4"/>
+      <c r="P49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q49" s="4"/>
-      <c r="S49" s="4"/>
+      <c r="S49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T49" s="4"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A50" s="6"/>
-      <c r="B50" s="1" t="s">
+      <c r="A50" s="1">
+        <v>41</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="G50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H50" s="4"/>
+      <c r="J50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K50" s="4"/>
+      <c r="M50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N50" s="4"/>
+      <c r="P50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q50" s="4"/>
+      <c r="S50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T50" s="4"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>42</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="G51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H51" s="4"/>
+      <c r="J51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K51" s="4"/>
+      <c r="M51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N51" s="4"/>
+      <c r="P51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q51" s="4"/>
+      <c r="S51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T51" s="4"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>43</v>
+      </c>
+      <c r="B52" s="4">
+        <v>1</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="G52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H52" s="4"/>
+      <c r="J52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K52" s="4"/>
+      <c r="M52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N52" s="4"/>
+      <c r="P52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q52" s="4"/>
+      <c r="S52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T52" s="4"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="G53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H53" s="4"/>
+      <c r="J53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K53" s="4"/>
+      <c r="M53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N53" s="4"/>
+      <c r="P53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q53" s="4"/>
+      <c r="S53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T53" s="4"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A55" s="6"/>
+      <c r="B55" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="9" t="s">
+      <c r="C55" s="10"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="9" t="s">
+      <c r="G55" s="1"/>
+      <c r="H55" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J50" s="1"/>
-      <c r="K50" s="9" t="s">
+      <c r="J55" s="1"/>
+      <c r="K55" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M50" s="1"/>
-      <c r="N50" s="9" t="s">
+      <c r="M55" s="1"/>
+      <c r="N55" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="9" t="s">
+      <c r="P55" s="1"/>
+      <c r="Q55" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S50" s="1"/>
-      <c r="T50" s="9" t="s">
+      <c r="S55" s="1"/>
+      <c r="T55" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J51" s="1"/>
-      <c r="K51" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M51" s="1"/>
-      <c r="N51" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S51" s="1"/>
-      <c r="T51" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" s="12">
-        <f>SUM(D10:D48)</f>
-        <v>70</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="12">
-        <f>SUM(G10:G48)</f>
-        <v>45</v>
-      </c>
-      <c r="J52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K52" s="12">
-        <f>SUM(J10:J48)</f>
-        <v>55</v>
-      </c>
-      <c r="M52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N52" s="12">
-        <f>SUM(M10:M48)</f>
-        <v>195</v>
-      </c>
-      <c r="P52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q52" s="12">
-        <f>SUM(P10:P48)</f>
-        <v>-30</v>
-      </c>
-      <c r="S52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T52" s="12">
-        <f>SUM(S10:S48)</f>
-        <v>-335</v>
-      </c>
-      <c r="U52" s="1">
-        <f>SUM(E52,H52,K52,N52,Q52,T52)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G56" s="1"/>
+      <c r="H56" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J56" s="1"/>
+      <c r="K56" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M56" s="1"/>
+      <c r="N56" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S56" s="1"/>
+      <c r="T56" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="12">
+        <f>SUM(D10:D53)</f>
+        <v>95</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="12">
+        <f>SUM(G10:G53)</f>
+        <v>50</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K57" s="12">
+        <f>SUM(J10:J53)</f>
+        <v>160</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N57" s="12">
+        <f>SUM(M10:M53)</f>
+        <v>170</v>
+      </c>
+      <c r="P57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q57" s="12">
+        <f>SUM(P10:P53)</f>
+        <v>-105</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T57" s="12">
+        <f>SUM(S10:S53)</f>
+        <v>-370</v>
+      </c>
+      <c r="U57" s="1">
+        <f>SUM(E57,H57,K57,N57,Q57,T57)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3156,7 +3437,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E52">
+  <conditionalFormatting sqref="E57">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3167,7 +3448,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K52">
+  <conditionalFormatting sqref="K57">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3178,7 +3459,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
+  <conditionalFormatting sqref="H57">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3189,7 +3470,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N52">
+  <conditionalFormatting sqref="N57">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3200,7 +3481,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T52">
+  <conditionalFormatting sqref="T57">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3211,7 +3492,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q52">
+  <conditionalFormatting sqref="Q57">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
New format for EBE dream 11.
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA20609-DFEA-AC40-BD88-1BF355909CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931B698A-7B9E-8B4A-8E0D-AEC6D8ECC9D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="460" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -891,8 +891,8 @@
   <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U57" sqref="U57"/>
+      <pane ySplit="8" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Contest 37 CSK vs RR
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931B698A-7B9E-8B4A-8E0D-AEC6D8ECC9D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A8BC4B-C157-6D40-80F3-F2973D5CB83D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="460" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Points</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>KXI vs SRH</t>
+  </si>
+  <si>
+    <t>RCB vs CSK</t>
+  </si>
+  <si>
+    <t>RR vs MI</t>
+  </si>
+  <si>
+    <t>KKR vs KXI</t>
   </si>
 </sst>
 </file>
@@ -888,11 +897,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U60" sqref="U60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2871,36 +2880,48 @@
       <c r="C44" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="3" t="str">
+      <c r="D44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="G44" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H44" s="4"/>
-      <c r="J44" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H44" s="4">
+        <v>100</v>
+      </c>
+      <c r="J44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K44" s="4"/>
-      <c r="M44" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K44" s="4">
+        <v>20</v>
+      </c>
+      <c r="M44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N44" s="4"/>
-      <c r="P44" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N44" s="4">
+        <v>40</v>
+      </c>
+      <c r="P44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q44" s="4"/>
-      <c r="S44" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>80</v>
+      </c>
+      <c r="S44" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T44" s="4"/>
+        <v>-10</v>
+      </c>
+      <c r="T44" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -2912,36 +2933,48 @@
       <c r="C45" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="3" t="str">
+      <c r="D45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E45" s="4"/>
-      <c r="G45" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E45" s="4">
+        <v>60</v>
+      </c>
+      <c r="G45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H45" s="4"/>
-      <c r="J45" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H45" s="4">
+        <v>100</v>
+      </c>
+      <c r="J45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K45" s="4"/>
-      <c r="M45" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K45" s="4">
+        <v>40</v>
+      </c>
+      <c r="M45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N45" s="4"/>
-      <c r="P45" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N45" s="4">
+        <v>0</v>
+      </c>
+      <c r="P45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q45" s="4"/>
-      <c r="S45" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>20</v>
+      </c>
+      <c r="S45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T45" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="T45" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -2953,36 +2986,48 @@
       <c r="C46" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="3" t="str">
+      <c r="D46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="G46" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E46" s="4">
+        <v>40</v>
+      </c>
+      <c r="G46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="J46" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H46" s="4">
+        <v>100</v>
+      </c>
+      <c r="J46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K46" s="4"/>
-      <c r="M46" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K46" s="4">
+        <v>60</v>
+      </c>
+      <c r="M46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N46" s="4"/>
-      <c r="P46" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N46" s="4">
+        <v>20</v>
+      </c>
+      <c r="P46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q46" s="4"/>
-      <c r="S46" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>80</v>
+      </c>
+      <c r="S46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T46" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T46" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -3231,194 +3276,296 @@
       <c r="T52" s="4"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="13"/>
+      <c r="A53" s="1">
+        <v>44</v>
+      </c>
+      <c r="B53" s="4">
+        <v>2</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="D53" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
         <v/>
       </c>
       <c r="E53" s="4"/>
       <c r="G53" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
         <v/>
       </c>
       <c r="H53" s="4"/>
       <c r="J53" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
         <v/>
       </c>
       <c r="K53" s="4"/>
       <c r="M53" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
         <v/>
       </c>
       <c r="N53" s="4"/>
       <c r="P53" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
         <v/>
       </c>
       <c r="Q53" s="4"/>
       <c r="S53" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
         <v/>
       </c>
       <c r="T53" s="4"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
+      <c r="A54" s="1">
+        <v>45</v>
+      </c>
+      <c r="B54" s="4">
+        <v>2</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(E54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E54" s="4"/>
-      <c r="G54" s="4"/>
+      <c r="G54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(H54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H54" s="4"/>
-      <c r="J54" s="4"/>
+      <c r="J54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(K54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K54" s="4"/>
-      <c r="M54" s="4"/>
+      <c r="M54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(N54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N54" s="4"/>
-      <c r="P54" s="4"/>
+      <c r="P54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(Q54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q54" s="4"/>
-      <c r="S54" s="4"/>
+      <c r="S54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(T54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T54" s="4"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A55" s="6"/>
-      <c r="B55" s="1" t="s">
+      <c r="A55" s="1">
+        <v>46</v>
+      </c>
+      <c r="B55" s="4">
+        <v>2</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(E55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="G55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(H55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H55" s="4"/>
+      <c r="J55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(K55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K55" s="4"/>
+      <c r="M55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(N55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N55" s="4"/>
+      <c r="P55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(Q55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q55" s="4"/>
+      <c r="S55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(T55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T55" s="4"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="G56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H56" s="4"/>
+      <c r="J56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K56" s="4"/>
+      <c r="M56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N56" s="4"/>
+      <c r="P56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q56" s="4"/>
+      <c r="S56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T56" s="4"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A58" s="6"/>
+      <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="9" t="s">
+      <c r="C58" s="10"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="9" t="s">
+      <c r="G58" s="1"/>
+      <c r="H58" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J55" s="1"/>
-      <c r="K55" s="9" t="s">
+      <c r="J58" s="1"/>
+      <c r="K58" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M55" s="1"/>
-      <c r="N55" s="9" t="s">
+      <c r="M58" s="1"/>
+      <c r="N58" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="9" t="s">
+      <c r="P58" s="1"/>
+      <c r="Q58" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S55" s="1"/>
-      <c r="T55" s="9" t="s">
+      <c r="S58" s="1"/>
+      <c r="T58" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J56" s="1"/>
-      <c r="K56" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M56" s="1"/>
-      <c r="N56" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S56" s="1"/>
-      <c r="T56" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" s="12">
-        <f>SUM(D10:D53)</f>
-        <v>95</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="12">
-        <f>SUM(G10:G53)</f>
-        <v>50</v>
-      </c>
-      <c r="J57" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K57" s="12">
-        <f>SUM(J10:J53)</f>
-        <v>160</v>
-      </c>
-      <c r="M57" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N57" s="12">
-        <f>SUM(M10:M53)</f>
-        <v>170</v>
-      </c>
-      <c r="P57" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q57" s="12">
-        <f>SUM(P10:P53)</f>
-        <v>-105</v>
-      </c>
-      <c r="S57" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T57" s="12">
-        <f>SUM(S10:S53)</f>
-        <v>-370</v>
-      </c>
-      <c r="U57" s="1">
-        <f>SUM(E57,H57,K57,N57,Q57,T57)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D59" s="1"/>
+      <c r="E59" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J59" s="1"/>
+      <c r="K59" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M59" s="1"/>
+      <c r="N59" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S59" s="1"/>
+      <c r="T59" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
+      <c r="D60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="12">
+        <f>SUM(D10:D56)</f>
+        <v>45</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="12">
+        <f>SUM(G10:G56)</f>
+        <v>200</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K60" s="12">
+        <f>SUM(J10:J56)</f>
+        <v>115</v>
+      </c>
+      <c r="M60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N60" s="12">
+        <f>SUM(M10:M56)</f>
+        <v>110</v>
+      </c>
+      <c r="P60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q60" s="12">
+        <f>SUM(P10:P56)</f>
+        <v>-85</v>
+      </c>
+      <c r="S60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T60" s="12">
+        <f>SUM(S10:S56)</f>
+        <v>-385</v>
+      </c>
+      <c r="U60" s="1">
+        <f>SUM(E60,H60,K60,N60,Q60,T60)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
@@ -3426,6 +3573,27 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3437,7 +3605,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E57">
+  <conditionalFormatting sqref="E60">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3448,7 +3616,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K57">
+  <conditionalFormatting sqref="K60">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3459,7 +3627,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57">
+  <conditionalFormatting sqref="H60">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3470,7 +3638,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57">
+  <conditionalFormatting sqref="N60">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3481,7 +3649,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T57">
+  <conditionalFormatting sqref="T60">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3492,7 +3660,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q57">
+  <conditionalFormatting sqref="Q60">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 38 KXI vs DC
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A8BC4B-C157-6D40-80F3-F2973D5CB83D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FBAD35-FFE6-3F41-8503-8F816875194F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="460" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>Points</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>KKR vs KXI</t>
+  </si>
+  <si>
+    <t>SRH vs DC</t>
   </si>
 </sst>
 </file>
@@ -897,11 +900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U64"/>
+  <dimension ref="A1:U65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U60" sqref="U60"/>
+      <selection pane="bottomLeft" activeCell="U61" sqref="U61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3039,36 +3042,48 @@
       <c r="C47" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="3" t="str">
+      <c r="D47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="G47" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E47" s="4">
+        <v>80</v>
+      </c>
+      <c r="G47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H47" s="4"/>
-      <c r="J47" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H47" s="4">
+        <v>20</v>
+      </c>
+      <c r="J47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K47" s="4"/>
-      <c r="M47" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K47" s="4">
+        <v>40</v>
+      </c>
+      <c r="M47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N47" s="4"/>
-      <c r="P47" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N47" s="4">
+        <v>100</v>
+      </c>
+      <c r="P47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q47" s="4"/>
-      <c r="S47" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>60</v>
+      </c>
+      <c r="S47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T47" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T47" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -3399,36 +3414,42 @@
       <c r="T55" s="4"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="13"/>
+      <c r="A56" s="1">
+        <v>46</v>
+      </c>
+      <c r="B56" s="4">
+        <v>2</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="D56" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
         <v/>
       </c>
       <c r="E56" s="4"/>
       <c r="G56" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
         <v/>
       </c>
       <c r="H56" s="4"/>
       <c r="J56" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
         <v/>
       </c>
       <c r="K56" s="4"/>
       <c r="M56" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
         <v/>
       </c>
       <c r="N56" s="4"/>
       <c r="P56" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
         <v/>
       </c>
       <c r="Q56" s="4"/>
       <c r="S56" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
         <v/>
       </c>
       <c r="T56" s="4"/>
@@ -3436,143 +3457,171 @@
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E57" s="4"/>
-      <c r="G57" s="4"/>
+      <c r="G57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="J57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K57" s="4"/>
-      <c r="M57" s="4"/>
+      <c r="M57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N57" s="4"/>
-      <c r="P57" s="4"/>
+      <c r="P57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q57" s="4"/>
-      <c r="S57" s="4"/>
+      <c r="S57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T57" s="4"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A58" s="6"/>
-      <c r="B58" s="1" t="s">
+      <c r="A58" s="1"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A59" s="6"/>
+      <c r="B59" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="10"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="9" t="s">
+      <c r="C59" s="10"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="9" t="s">
+      <c r="G59" s="1"/>
+      <c r="H59" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J58" s="1"/>
-      <c r="K58" s="9" t="s">
+      <c r="J59" s="1"/>
+      <c r="K59" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M58" s="1"/>
-      <c r="N58" s="9" t="s">
+      <c r="M59" s="1"/>
+      <c r="N59" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="9" t="s">
+      <c r="P59" s="1"/>
+      <c r="Q59" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S58" s="1"/>
-      <c r="T58" s="9" t="s">
+      <c r="S59" s="1"/>
+      <c r="T59" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J59" s="1"/>
-      <c r="K59" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M59" s="1"/>
-      <c r="N59" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S59" s="1"/>
-      <c r="T59" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
-      <c r="D60" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" s="12">
-        <f>SUM(D10:D56)</f>
-        <v>45</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H60" s="12">
-        <f>SUM(G10:G56)</f>
-        <v>200</v>
-      </c>
-      <c r="J60" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K60" s="12">
-        <f>SUM(J10:J56)</f>
-        <v>115</v>
-      </c>
-      <c r="M60" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N60" s="12">
-        <f>SUM(M10:M56)</f>
-        <v>110</v>
-      </c>
-      <c r="P60" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q60" s="12">
-        <f>SUM(P10:P56)</f>
-        <v>-85</v>
-      </c>
-      <c r="S60" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T60" s="12">
-        <f>SUM(S10:S56)</f>
-        <v>-385</v>
-      </c>
-      <c r="U60" s="1">
-        <f>SUM(E60,H60,K60,N60,Q60,T60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D60" s="1"/>
+      <c r="E60" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J60" s="1"/>
+      <c r="K60" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M60" s="1"/>
+      <c r="N60" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S60" s="1"/>
+      <c r="T60" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
+      <c r="D61" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="12">
+        <f>SUM(D10:D57)</f>
+        <v>65</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" s="12">
+        <f>SUM(G10:G57)</f>
+        <v>180</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K61" s="12">
+        <f>SUM(J10:J57)</f>
+        <v>100</v>
+      </c>
+      <c r="M61" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N61" s="12">
+        <f>SUM(M10:M57)</f>
+        <v>160</v>
+      </c>
+      <c r="P61" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q61" s="12">
+        <f>SUM(P10:P57)</f>
+        <v>-95</v>
+      </c>
+      <c r="S61" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T61" s="12">
+        <f>SUM(S10:S57)</f>
+        <v>-410</v>
+      </c>
+      <c r="U61" s="1">
+        <f>SUM(E61,H61,K61,N61,Q61,T61)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
@@ -3594,6 +3643,13 @@
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3605,7 +3661,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E60">
+  <conditionalFormatting sqref="E61">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3616,7 +3672,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K60">
+  <conditionalFormatting sqref="K61">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3627,7 +3683,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H60">
+  <conditionalFormatting sqref="H61">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3638,7 +3694,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N60">
+  <conditionalFormatting sqref="N61">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3649,7 +3705,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T60">
+  <conditionalFormatting sqref="T61">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3660,7 +3716,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q60">
+  <conditionalFormatting sqref="Q61">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Results: Contest 39 KKR vs RCB
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FBAD35-FFE6-3F41-8503-8F816875194F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12FBBE4-AB0D-C64C-873A-030840CC7DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="460" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>Points</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>SRH vs DC</t>
+  </si>
+  <si>
+    <t>MI vs RCB</t>
   </si>
 </sst>
 </file>
@@ -900,11 +903,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U65"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U61" sqref="U61"/>
+      <pane ySplit="8" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U62" sqref="U62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3095,36 +3098,48 @@
       <c r="C48" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D48" s="3" t="str">
+      <c r="D48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E48" s="4"/>
-      <c r="G48" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E48" s="4">
+        <v>100</v>
+      </c>
+      <c r="G48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H48" s="4"/>
-      <c r="J48" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H48" s="4">
+        <v>20</v>
+      </c>
+      <c r="J48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K48" s="4"/>
-      <c r="M48" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K48" s="4">
+        <v>40</v>
+      </c>
+      <c r="M48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N48" s="4"/>
-      <c r="P48" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N48" s="4">
+        <v>0</v>
+      </c>
+      <c r="P48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q48" s="4"/>
-      <c r="S48" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>60</v>
+      </c>
+      <c r="S48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T48" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="T48" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -3415,7 +3430,7 @@
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B56" s="4">
         <v>2</v>
@@ -3455,36 +3470,42 @@
       <c r="T56" s="4"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="13"/>
+      <c r="A57" s="1">
+        <v>48</v>
+      </c>
+      <c r="B57" s="4">
+        <v>2</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="D57" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
         <v/>
       </c>
       <c r="E57" s="4"/>
       <c r="G57" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
         <v/>
       </c>
       <c r="H57" s="4"/>
       <c r="J57" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
         <v/>
       </c>
       <c r="K57" s="4"/>
       <c r="M57" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
         <v/>
       </c>
       <c r="N57" s="4"/>
       <c r="P57" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
         <v/>
       </c>
       <c r="Q57" s="4"/>
       <c r="S57" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
         <v/>
       </c>
       <c r="T57" s="4"/>
@@ -3492,143 +3513,171 @@
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E58" s="4"/>
-      <c r="G58" s="4"/>
+      <c r="G58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H58" s="4"/>
-      <c r="J58" s="4"/>
+      <c r="J58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K58" s="4"/>
-      <c r="M58" s="4"/>
+      <c r="M58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N58" s="4"/>
-      <c r="P58" s="4"/>
+      <c r="P58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q58" s="4"/>
-      <c r="S58" s="4"/>
+      <c r="S58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T58" s="4"/>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A59" s="6"/>
-      <c r="B59" s="1" t="s">
+      <c r="A59" s="1"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A60" s="6"/>
+      <c r="B60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="9" t="s">
+      <c r="C60" s="10"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="9" t="s">
+      <c r="G60" s="1"/>
+      <c r="H60" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J59" s="1"/>
-      <c r="K59" s="9" t="s">
+      <c r="J60" s="1"/>
+      <c r="K60" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M59" s="1"/>
-      <c r="N59" s="9" t="s">
+      <c r="M60" s="1"/>
+      <c r="N60" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="9" t="s">
+      <c r="P60" s="1"/>
+      <c r="Q60" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S59" s="1"/>
-      <c r="T59" s="9" t="s">
+      <c r="S60" s="1"/>
+      <c r="T60" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J60" s="1"/>
-      <c r="K60" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M60" s="1"/>
-      <c r="N60" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S60" s="1"/>
-      <c r="T60" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
-      <c r="D61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="12">
-        <f>SUM(D10:D57)</f>
-        <v>65</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H61" s="12">
-        <f>SUM(G10:G57)</f>
-        <v>180</v>
-      </c>
-      <c r="J61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K61" s="12">
-        <f>SUM(J10:J57)</f>
-        <v>100</v>
-      </c>
-      <c r="M61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N61" s="12">
-        <f>SUM(M10:M57)</f>
-        <v>160</v>
-      </c>
-      <c r="P61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q61" s="12">
-        <f>SUM(P10:P57)</f>
-        <v>-95</v>
-      </c>
-      <c r="S61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T61" s="12">
-        <f>SUM(S10:S57)</f>
-        <v>-410</v>
-      </c>
-      <c r="U61" s="1">
-        <f>SUM(E61,H61,K61,N61,Q61,T61)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D61" s="1"/>
+      <c r="E61" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J61" s="1"/>
+      <c r="K61" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S61" s="1"/>
+      <c r="T61" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
+      <c r="D62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="12">
+        <f>SUM(D10:D58)</f>
+        <v>115</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" s="12">
+        <f>SUM(G10:G58)</f>
+        <v>160</v>
+      </c>
+      <c r="J62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K62" s="12">
+        <f>SUM(J10:J58)</f>
+        <v>85</v>
+      </c>
+      <c r="M62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N62" s="12">
+        <f>SUM(M10:M58)</f>
+        <v>135</v>
+      </c>
+      <c r="P62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q62" s="12">
+        <f>SUM(P10:P58)</f>
+        <v>-105</v>
+      </c>
+      <c r="S62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T62" s="12">
+        <f>SUM(S10:S58)</f>
+        <v>-390</v>
+      </c>
+      <c r="U62" s="1">
+        <f>SUM(E62,H62,K62,N62,Q62,T62)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
@@ -3650,6 +3699,13 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3661,7 +3717,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E61">
+  <conditionalFormatting sqref="E62">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3672,7 +3728,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K61">
+  <conditionalFormatting sqref="K62">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3683,7 +3739,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61">
+  <conditionalFormatting sqref="H62">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3694,7 +3750,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N61">
+  <conditionalFormatting sqref="N62">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3705,7 +3761,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T61">
+  <conditionalFormatting sqref="T62">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3716,7 +3772,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q61">
+  <conditionalFormatting sqref="Q62">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Results: Contest 40 RR vs SRH
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12FBBE4-AB0D-C64C-873A-030840CC7DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF36C2A-7C86-C840-905F-1D29BACD2544}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="460" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>Points</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>MI vs RCB</t>
+  </si>
+  <si>
+    <t>CSK vs KKR</t>
   </si>
 </sst>
 </file>
@@ -903,11 +906,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U66"/>
+  <dimension ref="A1:U67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U62" sqref="U62"/>
+      <selection pane="bottomLeft" activeCell="U63" sqref="U63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3151,36 +3154,48 @@
       <c r="C49" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="3" t="str">
+      <c r="D49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="G49" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H49" s="4"/>
-      <c r="J49" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H49" s="4">
+        <v>20</v>
+      </c>
+      <c r="J49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K49" s="4"/>
-      <c r="M49" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K49" s="4">
+        <v>40</v>
+      </c>
+      <c r="M49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N49" s="4"/>
-      <c r="P49" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N49" s="4">
+        <v>60</v>
+      </c>
+      <c r="P49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q49" s="4"/>
-      <c r="S49" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>100</v>
+      </c>
+      <c r="S49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T49" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="T49" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -3511,36 +3526,42 @@
       <c r="T57" s="4"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="13"/>
+      <c r="A58" s="1">
+        <v>49</v>
+      </c>
+      <c r="B58" s="4">
+        <v>2</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>69</v>
+      </c>
       <c r="D58" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
         <v/>
       </c>
       <c r="E58" s="4"/>
       <c r="G58" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
         <v/>
       </c>
       <c r="H58" s="4"/>
       <c r="J58" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
         <v/>
       </c>
       <c r="K58" s="4"/>
       <c r="M58" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
         <v/>
       </c>
       <c r="N58" s="4"/>
       <c r="P58" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
         <v/>
       </c>
       <c r="Q58" s="4"/>
       <c r="S58" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
         <v/>
       </c>
       <c r="T58" s="4"/>
@@ -3548,143 +3569,171 @@
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="E59" s="4"/>
-      <c r="G59" s="4"/>
+      <c r="G59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="H59" s="4"/>
-      <c r="J59" s="4"/>
+      <c r="J59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="K59" s="4"/>
-      <c r="M59" s="4"/>
+      <c r="M59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="N59" s="4"/>
-      <c r="P59" s="4"/>
+      <c r="P59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q59" s="4"/>
-      <c r="S59" s="4"/>
+      <c r="S59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
       <c r="T59" s="4"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A60" s="6"/>
-      <c r="B60" s="1" t="s">
+      <c r="A60" s="1"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A61" s="6"/>
+      <c r="B61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="10"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="9" t="s">
+      <c r="C61" s="10"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="9" t="s">
+      <c r="G61" s="1"/>
+      <c r="H61" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J60" s="1"/>
-      <c r="K60" s="9" t="s">
+      <c r="J61" s="1"/>
+      <c r="K61" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M60" s="1"/>
-      <c r="N60" s="9" t="s">
+      <c r="M61" s="1"/>
+      <c r="N61" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="9" t="s">
+      <c r="P61" s="1"/>
+      <c r="Q61" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S60" s="1"/>
-      <c r="T60" s="9" t="s">
+      <c r="S61" s="1"/>
+      <c r="T61" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J61" s="1"/>
-      <c r="K61" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M61" s="1"/>
-      <c r="N61" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S61" s="1"/>
-      <c r="T61" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
-      <c r="D62" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" s="12">
-        <f>SUM(D10:D58)</f>
-        <v>115</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H62" s="12">
-        <f>SUM(G10:G58)</f>
-        <v>160</v>
-      </c>
-      <c r="J62" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K62" s="12">
-        <f>SUM(J10:J58)</f>
-        <v>85</v>
-      </c>
-      <c r="M62" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N62" s="12">
-        <f>SUM(M10:M58)</f>
-        <v>135</v>
-      </c>
-      <c r="P62" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q62" s="12">
-        <f>SUM(P10:P58)</f>
-        <v>-105</v>
-      </c>
-      <c r="S62" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T62" s="12">
-        <f>SUM(S10:S58)</f>
-        <v>-390</v>
-      </c>
-      <c r="U62" s="1">
-        <f>SUM(E62,H62,K62,N62,Q62,T62)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D62" s="1"/>
+      <c r="E62" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="H62" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J62" s="1"/>
+      <c r="K62" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M62" s="1"/>
+      <c r="N62" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S62" s="1"/>
+      <c r="T62" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
+      <c r="D63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="12">
+        <f>SUM(D10:D59)</f>
+        <v>90</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" s="12">
+        <f>SUM(G10:G59)</f>
+        <v>140</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K63" s="12">
+        <f>SUM(J10:J59)</f>
+        <v>70</v>
+      </c>
+      <c r="M63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N63" s="12">
+        <f>SUM(M10:M59)</f>
+        <v>125</v>
+      </c>
+      <c r="P63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q63" s="12">
+        <f>SUM(P10:P59)</f>
+        <v>-55</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T63" s="12">
+        <f>SUM(S10:S59)</f>
+        <v>-370</v>
+      </c>
+      <c r="U63" s="1">
+        <f>SUM(E63,H63,K63,N63,Q63,T63)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
@@ -3706,6 +3755,13 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3717,7 +3773,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E62">
+  <conditionalFormatting sqref="E63">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3728,7 +3784,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
+  <conditionalFormatting sqref="K63">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3739,7 +3795,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H62">
+  <conditionalFormatting sqref="H63">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3750,7 +3806,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N62">
+  <conditionalFormatting sqref="N63">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3761,7 +3817,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T62">
+  <conditionalFormatting sqref="T63">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3772,7 +3828,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q62">
+  <conditionalFormatting sqref="Q63">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Results weekend - RR vs MI
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF36C2A-7C86-C840-905F-1D29BACD2544}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F4E918-38EE-6B4D-BA34-1746E291C0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="460" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2240" yWindow="520" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>Points</t>
   </si>
@@ -240,6 +240,27 @@
   </si>
   <si>
     <t>CSK vs KKR</t>
+  </si>
+  <si>
+    <t>KXI vs RR</t>
+  </si>
+  <si>
+    <t>DC vs MI</t>
+  </si>
+  <si>
+    <t>RCB vs SRH</t>
+  </si>
+  <si>
+    <t>CSK vs KXI</t>
+  </si>
+  <si>
+    <t>KKR vs RR</t>
+  </si>
+  <si>
+    <t>DC vs RCB</t>
+  </si>
+  <si>
+    <t>SRH vs MI</t>
   </si>
 </sst>
 </file>
@@ -906,11 +927,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U67"/>
+  <dimension ref="A1:U74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U63" sqref="U63"/>
+      <pane ySplit="8" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U70" sqref="U70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3144,7 +3165,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>40</v>
       </c>
@@ -3197,7 +3218,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>41</v>
       </c>
@@ -3207,38 +3228,50 @@
       <c r="C50" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D50" s="3" t="str">
+      <c r="D50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E50" s="4"/>
-      <c r="G50" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E50" s="4">
+        <v>20</v>
+      </c>
+      <c r="G50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H50" s="4"/>
-      <c r="J50" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H50" s="4">
+        <v>100</v>
+      </c>
+      <c r="J50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K50" s="4"/>
-      <c r="M50" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K50" s="4">
+        <v>60</v>
+      </c>
+      <c r="M50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N50" s="4"/>
-      <c r="P50" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N50" s="4">
+        <v>0</v>
+      </c>
+      <c r="P50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q50" s="4"/>
-      <c r="S50" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>40</v>
+      </c>
+      <c r="S50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T50" s="4"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="T50" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>42</v>
       </c>
@@ -3248,38 +3281,50 @@
       <c r="C51" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="3" t="str">
+      <c r="D51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="G51" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E51" s="4">
+        <v>20</v>
+      </c>
+      <c r="G51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H51" s="4"/>
-      <c r="J51" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H51" s="4">
+        <v>100</v>
+      </c>
+      <c r="J51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K51" s="4"/>
-      <c r="M51" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K51" s="4">
+        <v>80</v>
+      </c>
+      <c r="M51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N51" s="4"/>
-      <c r="P51" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N51" s="4">
+        <v>0</v>
+      </c>
+      <c r="P51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q51" s="4"/>
-      <c r="S51" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>60</v>
+      </c>
+      <c r="S51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T51" s="4"/>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-15</v>
+      </c>
+      <c r="T51" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43</v>
       </c>
@@ -3289,125 +3334,161 @@
       <c r="C52" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="3" t="str">
+      <c r="D52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="G52" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H52" s="4"/>
-      <c r="J52" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H52" s="4">
+        <v>100</v>
+      </c>
+      <c r="J52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K52" s="4"/>
-      <c r="M52" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K52" s="4">
+        <v>80</v>
+      </c>
+      <c r="M52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N52" s="4"/>
-      <c r="P52" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N52" s="4">
+        <v>60</v>
+      </c>
+      <c r="P52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q52" s="4"/>
-      <c r="S52" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>40</v>
+      </c>
+      <c r="S52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T52" s="4"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-20</v>
+      </c>
+      <c r="T52" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>44</v>
       </c>
       <c r="B53" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="3" t="str">
+      <c r="D53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E53" s="4"/>
-      <c r="G53" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H53" s="4"/>
-      <c r="J53" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H53" s="4">
+        <v>20</v>
+      </c>
+      <c r="J53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K53" s="4"/>
-      <c r="M53" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K53" s="4">
+        <v>100</v>
+      </c>
+      <c r="M53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N53" s="4"/>
-      <c r="P53" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N53" s="4">
+        <v>80</v>
+      </c>
+      <c r="P53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q53" s="4"/>
-      <c r="S53" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>60</v>
+      </c>
+      <c r="S53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE)),"",VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  score, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T53" s="4"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-15</v>
+      </c>
+      <c r="T53" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>45</v>
       </c>
       <c r="B54" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="3" t="str">
+      <c r="D54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(E54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="G54" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E54" s="4">
+        <v>20</v>
+      </c>
+      <c r="G54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(H54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H54" s="4"/>
-      <c r="J54" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H54" s="4">
+        <v>40</v>
+      </c>
+      <c r="J54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(K54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K54" s="4"/>
-      <c r="M54" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K54" s="4">
+        <v>100</v>
+      </c>
+      <c r="M54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(N54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N54" s="4"/>
-      <c r="P54" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N54" s="4">
+        <v>60</v>
+      </c>
+      <c r="P54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(Q54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q54" s="4"/>
-      <c r="S54" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>80</v>
+      </c>
+      <c r="S54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE)),"",VLOOKUP(RANK(T54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  score, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T54" s="4"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+        <v>-25</v>
+      </c>
+      <c r="T54" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>46</v>
       </c>
       <c r="B55" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>66</v>
@@ -3443,12 +3524,12 @@
       </c>
       <c r="T55" s="4"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>47</v>
       </c>
       <c r="B56" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>67</v>
@@ -3484,12 +3565,12 @@
       </c>
       <c r="T56" s="4"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>48</v>
       </c>
       <c r="B57" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>68</v>
@@ -3525,12 +3606,12 @@
       </c>
       <c r="T57" s="4"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>49</v>
       </c>
       <c r="B58" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>69</v>
@@ -3566,202 +3647,489 @@
       </c>
       <c r="T58" s="4"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="13"/>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>50</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>70</v>
+      </c>
       <c r="D59" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
         <v/>
       </c>
       <c r="E59" s="4"/>
       <c r="G59" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
         <v/>
       </c>
       <c r="H59" s="4"/>
       <c r="J59" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
         <v/>
       </c>
       <c r="K59" s="4"/>
       <c r="M59" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
         <v/>
       </c>
       <c r="N59" s="4"/>
       <c r="P59" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
         <v/>
       </c>
       <c r="Q59" s="4"/>
       <c r="S59" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
         <v/>
       </c>
       <c r="T59" s="4"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A60" s="1"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>51</v>
+      </c>
+      <c r="B60" s="4">
+        <v>1</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(E60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E60" s="4"/>
-      <c r="G60" s="4"/>
+      <c r="G60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(H60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H60" s="4"/>
-      <c r="J60" s="4"/>
+      <c r="J60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(K60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K60" s="4"/>
-      <c r="M60" s="4"/>
+      <c r="M60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(N60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N60" s="4"/>
-      <c r="P60" s="4"/>
+      <c r="P60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(Q60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q60" s="4"/>
-      <c r="S60" s="4"/>
+      <c r="S60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(T60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T60" s="4"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A61" s="6"/>
-      <c r="B61" s="1" t="s">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>52</v>
+      </c>
+      <c r="B61" s="4">
+        <v>1</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(E61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E61" s="4"/>
+      <c r="G61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(H61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H61" s="4"/>
+      <c r="J61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(K61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K61" s="4"/>
+      <c r="M61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(N61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N61" s="4"/>
+      <c r="P61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(Q61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q61" s="4"/>
+      <c r="S61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(T61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T61" s="4"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>53</v>
+      </c>
+      <c r="B62" s="4">
+        <v>1</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(E62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E62" s="4"/>
+      <c r="G62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(H62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H62" s="4"/>
+      <c r="J62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(K62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K62" s="4"/>
+      <c r="M62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(N62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N62" s="4"/>
+      <c r="P62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(Q62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q62" s="4"/>
+      <c r="S62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(T62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T62" s="4"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>54</v>
+      </c>
+      <c r="B63" s="4">
+        <v>1</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(E63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="G63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(H63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H63" s="4"/>
+      <c r="J63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(K63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K63" s="4"/>
+      <c r="M63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(N63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N63" s="4"/>
+      <c r="P63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(Q63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q63" s="4"/>
+      <c r="S63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(T63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T63" s="4"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>55</v>
+      </c>
+      <c r="B64" s="4">
+        <v>1</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE)),"",VLOOKUP(RANK(E64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E64" s="4"/>
+      <c r="G64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE)),"",VLOOKUP(RANK(H64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="J64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE)),"",VLOOKUP(RANK(K64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K64" s="4"/>
+      <c r="M64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE)),"",VLOOKUP(RANK(N64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N64" s="4"/>
+      <c r="P64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE)),"",VLOOKUP(RANK(Q64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q64" s="4"/>
+      <c r="S64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE)),"",VLOOKUP(RANK(T64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  score, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T64" s="4"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>56</v>
+      </c>
+      <c r="B65" s="4">
+        <v>1</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE)),"",VLOOKUP(RANK(E65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E65" s="4"/>
+      <c r="G65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE)),"",VLOOKUP(RANK(H65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H65" s="4"/>
+      <c r="J65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE)),"",VLOOKUP(RANK(K65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K65" s="4"/>
+      <c r="M65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE)),"",VLOOKUP(RANK(N65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N65" s="4"/>
+      <c r="P65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE)),"",VLOOKUP(RANK(Q65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q65" s="4"/>
+      <c r="S65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE)),"",VLOOKUP(RANK(T65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  score, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T65" s="4"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E66" s="4"/>
+      <c r="G66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H66" s="4"/>
+      <c r="J66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K66" s="4"/>
+      <c r="M66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N66" s="4"/>
+      <c r="P66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q66" s="4"/>
+      <c r="S66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, 2, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T66" s="4"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A68" s="6"/>
+      <c r="B68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="10"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="9" t="s">
+      <c r="C68" s="10"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="9" t="s">
+      <c r="G68" s="1"/>
+      <c r="H68" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J61" s="1"/>
-      <c r="K61" s="9" t="s">
+      <c r="J68" s="1"/>
+      <c r="K68" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M61" s="1"/>
-      <c r="N61" s="9" t="s">
+      <c r="M68" s="1"/>
+      <c r="N68" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="9" t="s">
+      <c r="P68" s="1"/>
+      <c r="Q68" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S61" s="1"/>
-      <c r="T61" s="9" t="s">
+      <c r="S68" s="1"/>
+      <c r="T68" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="11" t="str">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="11" t="str">
         <f>D9</f>
         <v>Anantha</v>
       </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="11" t="str">
+      <c r="G69" s="1"/>
+      <c r="H69" s="11" t="str">
         <f>G9</f>
         <v>Jayanth</v>
       </c>
-      <c r="J62" s="1"/>
-      <c r="K62" s="11" t="str">
+      <c r="J69" s="1"/>
+      <c r="K69" s="11" t="str">
         <f>J9</f>
         <v>Justin</v>
       </c>
-      <c r="M62" s="1"/>
-      <c r="N62" s="11" t="str">
+      <c r="M69" s="1"/>
+      <c r="N69" s="11" t="str">
         <f>M9</f>
         <v>Rapaka</v>
       </c>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="11" t="str">
+      <c r="P69" s="1"/>
+      <c r="Q69" s="11" t="str">
         <f>P9</f>
         <v>Sushma</v>
       </c>
-      <c r="S62" s="1"/>
-      <c r="T62" s="11" t="str">
+      <c r="S69" s="1"/>
+      <c r="T69" s="11" t="str">
         <f>S9</f>
         <v>Sampath M</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="7" t="s">
+    <row r="70" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E63" s="12">
-        <f>SUM(D10:D59)</f>
-        <v>90</v>
-      </c>
-      <c r="G63" s="7" t="s">
+      <c r="E70" s="12">
+        <f>SUM(D10:D66)</f>
+        <v>-20</v>
+      </c>
+      <c r="G70" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H63" s="12">
-        <f>SUM(G10:G59)</f>
-        <v>140</v>
-      </c>
-      <c r="J63" s="7" t="s">
+      <c r="H70" s="12">
+        <f>SUM(G10:G66)</f>
+        <v>255</v>
+      </c>
+      <c r="J70" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K63" s="12">
-        <f>SUM(J10:J59)</f>
-        <v>70</v>
-      </c>
-      <c r="M63" s="7" t="s">
+      <c r="K70" s="12">
+        <f>SUM(J10:J66)</f>
+        <v>200</v>
+      </c>
+      <c r="M70" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N63" s="12">
-        <f>SUM(M10:M59)</f>
-        <v>125</v>
-      </c>
-      <c r="P63" s="7" t="s">
+      <c r="N70" s="12">
+        <f>SUM(M10:M66)</f>
+        <v>75</v>
+      </c>
+      <c r="P70" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q63" s="12">
-        <f>SUM(P10:P59)</f>
-        <v>-55</v>
-      </c>
-      <c r="S63" s="7" t="s">
+      <c r="Q70" s="12">
+        <f>SUM(P10:P66)</f>
+        <v>-85</v>
+      </c>
+      <c r="S70" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T63" s="12">
-        <f>SUM(S10:S59)</f>
-        <v>-370</v>
-      </c>
-      <c r="U63" s="1">
-        <f>SUM(E63,H63,K63,N63,Q63,T63)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
+      <c r="T70" s="12">
+        <f>SUM(S10:S66)</f>
+        <v>-425</v>
+      </c>
+      <c r="U70" s="1">
+        <f>SUM(E70,H70,K70,N70,Q70,T70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3773,7 +4141,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E63">
+  <conditionalFormatting sqref="E70">
     <cfRule type="cellIs" dxfId="17" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3784,7 +4152,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
+  <conditionalFormatting sqref="K70">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3795,7 +4163,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
+  <conditionalFormatting sqref="H70">
     <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3806,7 +4174,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N63">
+  <conditionalFormatting sqref="N70">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3817,7 +4185,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T63">
+  <conditionalFormatting sqref="T70">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3828,7 +4196,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q63">
+  <conditionalFormatting sqref="Q70">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Results contest 46 KKR vs KXI
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F4E918-38EE-6B4D-BA34-1746E291C0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A626673C-8775-B943-BEFD-B1ED8D79E7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="520" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2060" yWindow="700" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3493,36 +3493,48 @@
       <c r="C55" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D55" s="3" t="str">
+      <c r="D55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(E55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="G55" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E55" s="4">
+        <v>80</v>
+      </c>
+      <c r="G55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(H55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H55" s="4"/>
-      <c r="J55" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H55" s="4">
+        <v>40</v>
+      </c>
+      <c r="J55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(K55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K55" s="4"/>
-      <c r="M55" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K55" s="4">
+        <v>100</v>
+      </c>
+      <c r="M55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(N55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N55" s="4"/>
-      <c r="P55" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N55" s="4">
+        <v>60</v>
+      </c>
+      <c r="P55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(Q55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q55" s="4"/>
-      <c r="S55" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>0</v>
+      </c>
+      <c r="S55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE)),"",VLOOKUP(RANK(T55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  score, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T55" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T55" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -4061,42 +4073,42 @@
       </c>
       <c r="E70" s="12">
         <f>SUM(D10:D66)</f>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H70" s="12">
         <f>SUM(G10:G66)</f>
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="J70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K70" s="12">
         <f>SUM(J10:J66)</f>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N70" s="12">
         <f>SUM(M10:M66)</f>
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="P70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q70" s="12">
         <f>SUM(P10:P66)</f>
-        <v>-85</v>
+        <v>-110</v>
       </c>
       <c r="S70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="T70" s="12">
         <f>SUM(S10:S66)</f>
-        <v>-425</v>
+        <v>-445</v>
       </c>
       <c r="U70" s="1">
         <f>SUM(E70,H70,K70,N70,Q70,T70)</f>

</xml_diff>

<commit_message>
results till 49 MI vs RCB
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A626673C-8775-B943-BEFD-B1ED8D79E7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953A9DF9-5313-DF44-B478-E301C09BCD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="700" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3546,36 +3546,46 @@
       <c r="C56" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D56" s="3" t="str">
+      <c r="D56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E56" s="4"/>
-      <c r="G56" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E56" s="4">
+        <v>80</v>
+      </c>
+      <c r="G56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H56" s="4"/>
-      <c r="J56" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H56" s="4">
+        <v>40</v>
+      </c>
+      <c r="J56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K56" s="4"/>
-      <c r="M56" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N56" s="4"/>
-      <c r="P56" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K56" s="4">
+        <v>60</v>
+      </c>
+      <c r="M56" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="N56" s="4">
+        <v>20</v>
+      </c>
+      <c r="P56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q56" s="4"/>
-      <c r="S56" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE)),"",VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  score, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T56" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>100</v>
+      </c>
+      <c r="S56" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="T56" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -3587,36 +3597,46 @@
       <c r="C57" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D57" s="3" t="str">
+      <c r="D57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E57" s="4"/>
-      <c r="G57" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H57" s="4"/>
-      <c r="J57" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E57" s="4">
+        <v>20</v>
+      </c>
+      <c r="G57" s="3">
+        <v>35</v>
+      </c>
+      <c r="H57" s="4">
+        <v>100</v>
+      </c>
+      <c r="J57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K57" s="4"/>
-      <c r="M57" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N57" s="4"/>
-      <c r="P57" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K57" s="4">
+        <v>40</v>
+      </c>
+      <c r="M57" s="3">
+        <v>35</v>
+      </c>
+      <c r="N57" s="4">
+        <v>100</v>
+      </c>
+      <c r="P57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q57" s="4"/>
-      <c r="S57" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q57" s="4">
+        <v>60</v>
+      </c>
+      <c r="S57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE)),"",VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  score, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T57" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T57" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -4080,35 +4100,35 @@
       </c>
       <c r="H70" s="12">
         <f>SUM(G10:G66)</f>
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="J70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K70" s="12">
         <f>SUM(J10:J66)</f>
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="M70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N70" s="12">
         <f>SUM(M10:M66)</f>
-        <v>65</v>
+        <v>77.5</v>
       </c>
       <c r="P70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q70" s="12">
         <f>SUM(P10:P66)</f>
-        <v>-110</v>
+        <v>-70</v>
       </c>
       <c r="S70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="T70" s="12">
         <f>SUM(S10:S66)</f>
-        <v>-445</v>
+        <v>-492.5</v>
       </c>
       <c r="U70" s="1">
         <f>SUM(E70,H70,K70,N70,Q70,T70)</f>

</xml_diff>

<commit_message>
Results and playoffs rules.
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953A9DF9-5313-DF44-B478-E301C09BCD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62538C0C-83B6-1243-B83A-DAF7F1CAFF22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="700" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2260" yWindow="620" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3648,36 +3648,48 @@
       <c r="C58" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D58" s="3" t="str">
+      <c r="D58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E58" s="4"/>
-      <c r="G58" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E58" s="4">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H58" s="4"/>
-      <c r="J58" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H58" s="4">
+        <v>20</v>
+      </c>
+      <c r="J58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K58" s="4"/>
-      <c r="M58" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K58" s="4">
+        <v>80</v>
+      </c>
+      <c r="M58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N58" s="4"/>
-      <c r="P58" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N58" s="4">
+        <v>100</v>
+      </c>
+      <c r="P58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q58" s="4"/>
-      <c r="S58" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q58" s="4">
+        <v>40</v>
+      </c>
+      <c r="S58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE)),"",VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  score, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T58" s="4"/>
+        <v>-10</v>
+      </c>
+      <c r="T58" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -4093,42 +4105,42 @@
       </c>
       <c r="E70" s="12">
         <f>SUM(D10:D66)</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H70" s="12">
         <f>SUM(G10:G66)</f>
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="J70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K70" s="12">
         <f>SUM(J10:J66)</f>
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="M70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N70" s="12">
         <f>SUM(M10:M66)</f>
-        <v>77.5</v>
+        <v>127.5</v>
       </c>
       <c r="P70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q70" s="12">
         <f>SUM(P10:P66)</f>
-        <v>-70</v>
+        <v>-85</v>
       </c>
       <c r="S70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="T70" s="12">
         <f>SUM(S10:S66)</f>
-        <v>-492.5</v>
+        <v>-502.5</v>
       </c>
       <c r="U70" s="1">
         <f>SUM(E70,H70,K70,N70,Q70,T70)</f>

</xml_diff>

<commit_message>
Results before the fate of RCB for they meet againtst DC.
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62538C0C-83B6-1243-B83A-DAF7F1CAFF22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5E3EBB-42CC-4147-A972-50522B74AD4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="620" windowWidth="33260" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="4740" yWindow="960" windowWidth="29700" windowHeight="20500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -930,7 +930,7 @@
   <dimension ref="A1:U74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U70" sqref="U70"/>
     </sheetView>
   </sheetViews>
@@ -3701,36 +3701,46 @@
       <c r="C59" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D59" s="3" t="str">
+      <c r="D59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E59" s="4"/>
-      <c r="G59" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H59" s="4"/>
-      <c r="J59" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K59" s="4"/>
-      <c r="M59" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <v>-12.5</v>
+      </c>
+      <c r="H59" s="4">
+        <v>60</v>
+      </c>
+      <c r="J59" s="3">
+        <v>-12.5</v>
+      </c>
+      <c r="K59" s="4">
+        <v>60</v>
+      </c>
+      <c r="M59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N59" s="4"/>
-      <c r="P59" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N59" s="4">
+        <v>100</v>
+      </c>
+      <c r="P59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q59" s="4"/>
-      <c r="S59" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q59" s="4">
+        <v>80</v>
+      </c>
+      <c r="S59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE)),"",VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  score, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T59" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T59" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
@@ -3742,36 +3752,48 @@
       <c r="C60" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="3" t="str">
+      <c r="D60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(E60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E60" s="4"/>
-      <c r="G60" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E60" s="4">
+        <v>20</v>
+      </c>
+      <c r="G60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(H60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H60" s="4"/>
-      <c r="J60" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H60" s="4">
+        <v>80</v>
+      </c>
+      <c r="J60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(K60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K60" s="4"/>
-      <c r="M60" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K60" s="4">
+        <v>60</v>
+      </c>
+      <c r="M60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(N60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N60" s="4"/>
-      <c r="P60" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N60" s="4">
+        <v>100</v>
+      </c>
+      <c r="P60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(Q60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q60" s="4"/>
-      <c r="S60" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q60" s="4">
+        <v>40</v>
+      </c>
+      <c r="S60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE)),"",VLOOKUP(RANK(T60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  score, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T60" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T60" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -3783,36 +3805,46 @@
       <c r="C61" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D61" s="3" t="str">
+      <c r="D61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(E61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E61" s="4"/>
-      <c r="G61" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(H61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H61" s="4"/>
-      <c r="J61" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E61" s="4">
+        <v>40</v>
+      </c>
+      <c r="G61" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="H61" s="4">
+        <v>20</v>
+      </c>
+      <c r="J61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(K61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K61" s="4"/>
-      <c r="M61" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(N61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N61" s="4"/>
-      <c r="P61" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K61" s="4">
+        <v>60</v>
+      </c>
+      <c r="M61" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="N61" s="4">
+        <v>20</v>
+      </c>
+      <c r="P61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(Q61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q61" s="4"/>
-      <c r="S61" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q61" s="4">
+        <v>100</v>
+      </c>
+      <c r="S61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE)),"",VLOOKUP(RANK(T61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  score, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T61" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="T61" s="4">
+        <v>80</v>
+      </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -3824,36 +3856,48 @@
       <c r="C62" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D62" s="3" t="str">
+      <c r="D62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(E62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E62" s="4"/>
-      <c r="G62" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E62" s="4">
+        <v>20</v>
+      </c>
+      <c r="G62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(H62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H62" s="4"/>
-      <c r="J62" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H62" s="4">
+        <v>80</v>
+      </c>
+      <c r="J62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(K62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K62" s="4"/>
-      <c r="M62" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K62" s="4">
+        <v>40</v>
+      </c>
+      <c r="M62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(N62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N62" s="4"/>
-      <c r="P62" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N62" s="4">
+        <v>100</v>
+      </c>
+      <c r="P62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(Q62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q62" s="4"/>
-      <c r="S62" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q62" s="4">
+        <v>60</v>
+      </c>
+      <c r="S62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE)),"",VLOOKUP(RANK(T62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  score, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T62" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T62" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -3865,36 +3909,48 @@
       <c r="C63" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D63" s="3" t="str">
+      <c r="D63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(E63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E63" s="4"/>
-      <c r="G63" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E63" s="4">
+        <v>0</v>
+      </c>
+      <c r="G63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(H63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H63" s="4"/>
-      <c r="J63" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H63" s="4">
+        <v>40</v>
+      </c>
+      <c r="J63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(K63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K63" s="4"/>
-      <c r="M63" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K63" s="4">
+        <v>60</v>
+      </c>
+      <c r="M63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(N63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N63" s="4"/>
-      <c r="P63" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N63" s="4">
+        <v>80</v>
+      </c>
+      <c r="P63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(Q63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q63" s="4"/>
-      <c r="S63" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q63" s="4">
+        <v>20</v>
+      </c>
+      <c r="S63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE)),"",VLOOKUP(RANK(T63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  score, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T63" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="T63" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
@@ -4105,35 +4161,35 @@
       </c>
       <c r="E70" s="12">
         <f>SUM(D10:D66)</f>
-        <v>-25</v>
+        <v>-130</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H70" s="12">
         <f>SUM(G10:G66)</f>
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="J70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K70" s="12">
         <f>SUM(J10:J66)</f>
-        <v>245</v>
+        <v>187.5</v>
       </c>
       <c r="M70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N70" s="12">
         <f>SUM(M10:M66)</f>
-        <v>127.5</v>
+        <v>275</v>
       </c>
       <c r="P70" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q70" s="12">
         <f>SUM(P10:P66)</f>
-        <v>-85</v>
+        <v>-60</v>
       </c>
       <c r="S70" s="7" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
qualifier 1 completed with predictions
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C9F49A-4F7B-4441-83EC-F9EA4E689D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FDAE88-3341-AF4E-96AA-AECD5D1AD68C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="840" windowWidth="29700" windowHeight="21440" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="4980" yWindow="520" windowWidth="29700" windowHeight="21840" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4801,36 +4801,48 @@
       <c r="C66" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D66" s="3" t="str">
+      <c r="D66" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE)),"",VLOOKUP(RANK(E66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E66" s="4"/>
-      <c r="G66" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E66" s="4">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE)),"",VLOOKUP(RANK(H66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H66" s="4"/>
-      <c r="J66" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H66" s="4">
+        <v>80</v>
+      </c>
+      <c r="J66" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE)),"",VLOOKUP(RANK(K66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K66" s="4"/>
-      <c r="M66" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K66" s="4">
+        <v>100</v>
+      </c>
+      <c r="M66" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE)),"",VLOOKUP(RANK(N66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N66" s="4"/>
-      <c r="P66" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N66" s="4">
+        <v>20</v>
+      </c>
+      <c r="P66" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE)),"",VLOOKUP(RANK(Q66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q66" s="4"/>
-      <c r="S66" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q66" s="4">
+        <v>40</v>
+      </c>
+      <c r="S66" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE)),"",VLOOKUP(RANK(T66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  score, $B66+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T66" s="4"/>
+        <v>-10</v>
+      </c>
+      <c r="T66" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
@@ -5043,42 +5055,42 @@
       </c>
       <c r="E73" s="12">
         <f>SUM(D10:D69)</f>
-        <v>-95</v>
+        <v>-120</v>
       </c>
       <c r="G73" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H73" s="12">
         <f>SUM(G10:G69)</f>
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="J73" s="7" t="s">
         <v>13</v>
       </c>
       <c r="K73" s="12">
         <f>SUM(J10:J69)</f>
-        <v>182.5</v>
+        <v>232.5</v>
       </c>
       <c r="M73" s="7" t="s">
         <v>13</v>
       </c>
       <c r="N73" s="12">
         <f>SUM(M10:M69)</f>
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="P73" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q73" s="12">
         <f>SUM(P10:P69)</f>
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="S73" s="7" t="s">
         <v>13</v>
       </c>
       <c r="T73" s="12">
         <f>SUM(S10:S69)</f>
-        <v>-537.5</v>
+        <v>-547.5</v>
       </c>
       <c r="U73" s="1">
         <f>SUM(E73,H73,K73,N73,Q73,T73)</f>
@@ -5171,34 +5183,37 @@
       <c r="B81" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C81" s="1"/>
+      <c r="C81" s="1">
+        <v>0</v>
+      </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1">
-        <v>2</v>
+        <f>SUM(C81:F81)</f>
+        <v>0</v>
       </c>
       <c r="L81" s="35" t="s">
         <v>5</v>
       </c>
       <c r="M81" s="12">
         <f>E73</f>
-        <v>-95</v>
+        <v>-120</v>
       </c>
       <c r="N81" s="36">
         <v>-120</v>
       </c>
       <c r="O81" s="12">
         <f>G81</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P81" s="12">
         <f>(-SUM($N$81:$N$86)/SUM($O$81:$O$86))*O81</f>
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="Q81" s="12">
         <f>SUM(M81,N81,P81)</f>
-        <v>145</v>
+        <v>-240</v>
       </c>
       <c r="R81" s="32" t="s">
         <v>5</v>
@@ -5208,32 +5223,37 @@
       <c r="B82" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C82" s="1"/>
+      <c r="C82" s="1">
+        <v>0</v>
+      </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
+      <c r="G82" s="1">
+        <f t="shared" ref="G82:G86" si="0">SUM(C82:F82)</f>
+        <v>0</v>
+      </c>
       <c r="L82" s="35" t="s">
         <v>6</v>
       </c>
       <c r="M82" s="12">
         <f>H73</f>
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="N82" s="36">
         <v>-120</v>
       </c>
       <c r="O82" s="12">
-        <f t="shared" ref="O82:O85" si="0">G82</f>
+        <f t="shared" ref="O82:O85" si="1">G82</f>
         <v>0</v>
       </c>
       <c r="P82" s="12">
-        <f t="shared" ref="P82:P86" si="1">(-SUM($N$81:$N$86)/SUM($O$81:$O$86))*O82</f>
+        <f t="shared" ref="P82:P86" si="2">(-SUM($N$81:$N$86)/SUM($O$81:$O$86))*O82</f>
         <v>0</v>
       </c>
       <c r="Q82" s="12">
-        <f t="shared" ref="Q82:Q85" si="2">SUM(M82,N82,P82)</f>
-        <v>75</v>
+        <f t="shared" ref="Q82:Q85" si="3">SUM(M82,N82,P82)</f>
+        <v>95</v>
       </c>
       <c r="R82" s="32" t="s">
         <v>6</v>
@@ -5243,32 +5263,37 @@
       <c r="B83" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C83" s="1"/>
+      <c r="C83" s="1">
+        <v>10</v>
+      </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
+      <c r="G83" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="L83" s="35" t="s">
         <v>7</v>
       </c>
       <c r="M83" s="12">
         <f>K73</f>
-        <v>182.5</v>
+        <v>232.5</v>
       </c>
       <c r="N83" s="36">
         <v>-120</v>
       </c>
       <c r="O83" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="P83" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>313.04347826086956</v>
       </c>
       <c r="Q83" s="12">
-        <f t="shared" si="2"/>
-        <v>62.5</v>
+        <f t="shared" si="3"/>
+        <v>425.54347826086956</v>
       </c>
       <c r="R83" s="32" t="s">
         <v>7</v>
@@ -5278,32 +5303,37 @@
       <c r="B84" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C84" s="1"/>
+      <c r="C84" s="1">
+        <v>7</v>
+      </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
+      <c r="G84" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="L84" s="35" t="s">
         <v>8</v>
       </c>
       <c r="M84" s="12">
         <f>N73</f>
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="N84" s="36">
         <v>-120</v>
       </c>
       <c r="O84" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="P84" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>219.13043478260869</v>
       </c>
       <c r="Q84" s="12">
-        <f t="shared" si="2"/>
-        <v>125</v>
+        <f t="shared" si="3"/>
+        <v>324.13043478260869</v>
       </c>
       <c r="R84" s="32" t="s">
         <v>8</v>
@@ -5313,34 +5343,37 @@
       <c r="B85" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C85" s="1"/>
+      <c r="C85" s="1">
+        <v>3</v>
+      </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="L85" s="35" t="s">
         <v>9</v>
       </c>
       <c r="M85" s="12">
         <f>Q73</f>
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="N85" s="36">
         <v>-120</v>
       </c>
       <c r="O85" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="P85" s="12">
-        <f t="shared" si="1"/>
-        <v>180</v>
+        <f t="shared" si="2"/>
+        <v>93.913043478260875</v>
       </c>
       <c r="Q85" s="12">
-        <f t="shared" si="2"/>
-        <v>70</v>
+        <f t="shared" si="3"/>
+        <v>-31.086956521739125</v>
       </c>
       <c r="R85" s="32" t="s">
         <v>9</v>
@@ -5350,34 +5383,37 @@
       <c r="B86" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="1"/>
+      <c r="C86" s="1">
+        <v>3</v>
+      </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="L86" s="35" t="s">
         <v>10</v>
       </c>
       <c r="M86" s="12">
         <f>T73</f>
-        <v>-537.5</v>
+        <v>-547.5</v>
       </c>
       <c r="N86" s="36">
         <v>-120</v>
       </c>
       <c r="O86" s="12">
-        <f t="shared" ref="O86" si="3">G86</f>
-        <v>1</v>
+        <f t="shared" ref="O86" si="4">G86</f>
+        <v>3</v>
       </c>
       <c r="P86" s="12">
-        <f t="shared" si="1"/>
-        <v>180</v>
+        <f t="shared" si="2"/>
+        <v>93.913043478260875</v>
       </c>
       <c r="Q86" s="12">
-        <f t="shared" ref="Q86" si="4">SUM(M86,N86,P86)</f>
-        <v>-477.5</v>
+        <f t="shared" ref="Q86" si="5">SUM(M86,N86,P86)</f>
+        <v>-573.58695652173913</v>
       </c>
       <c r="R86" s="32" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Finals MI vs DC. Until next year.
</commit_message>
<xml_diff>
--- a/AFA 2020.xlsx
+++ b/AFA 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/IPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FDAE88-3341-AF4E-96AA-AECD5D1AD68C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE2F31A-D303-804A-B6E5-D53E53F5D64C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="520" windowWidth="29700" windowHeight="21840" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="5020" yWindow="560" windowWidth="30120" windowHeight="21840" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="112">
   <si>
     <t>Points</t>
   </si>
@@ -353,6 +353,21 @@
   </si>
   <si>
     <t>Winner Prediction - Coins</t>
+  </si>
+  <si>
+    <t>Eliminator SRH vs RCB</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Qualifier 2 DC vs SRH</t>
+  </si>
+  <si>
+    <t>Finals MI vs DC</t>
+  </si>
+  <si>
+    <t>Congrats</t>
   </si>
 </sst>
 </file>
@@ -661,7 +676,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -736,6 +751,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -744,307 +762,7 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1655,11 +1373,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U87"/>
+  <dimension ref="A1:U86"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q87" sqref="Q87"/>
+      <selection pane="bottomLeft" activeCell="Q86" sqref="Q86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4854,36 +4572,48 @@
       <c r="C67" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="3" t="str">
+      <c r="D67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE)),"",VLOOKUP(RANK(E67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E67" s="4"/>
-      <c r="G67" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E67" s="4">
+        <v>20</v>
+      </c>
+      <c r="G67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE)),"",VLOOKUP(RANK(H67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H67" s="4"/>
-      <c r="J67" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H67" s="4">
+        <v>0</v>
+      </c>
+      <c r="J67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE)),"",VLOOKUP(RANK(K67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K67" s="4"/>
-      <c r="M67" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K67" s="4">
+        <v>40</v>
+      </c>
+      <c r="M67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE)),"",VLOOKUP(RANK(N67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N67" s="4"/>
-      <c r="P67" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N67" s="4">
+        <v>80</v>
+      </c>
+      <c r="P67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE)),"",VLOOKUP(RANK(Q67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q67" s="4"/>
-      <c r="S67" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q67" s="4">
+        <v>100</v>
+      </c>
+      <c r="S67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE)),"",VLOOKUP(RANK(T67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  score, $B67+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T67" s="4"/>
+        <v>-10</v>
+      </c>
+      <c r="T67" s="4">
+        <v>60</v>
+      </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -4892,37 +4622,51 @@
       <c r="B68" s="4">
         <v>1</v>
       </c>
-      <c r="C68" s="13"/>
-      <c r="D68" s="3" t="str">
+      <c r="C68" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE)),"",VLOOKUP(RANK(E68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E68" s="4"/>
-      <c r="G68" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E68" s="4">
+        <v>60</v>
+      </c>
+      <c r="G68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE)),"",VLOOKUP(RANK(H68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H68" s="4"/>
-      <c r="J68" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H68" s="4">
+        <v>80</v>
+      </c>
+      <c r="J68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE)),"",VLOOKUP(RANK(K68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K68" s="4"/>
-      <c r="M68" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K68" s="4">
+        <v>20</v>
+      </c>
+      <c r="M68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE)),"",VLOOKUP(RANK(N68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N68" s="4"/>
-      <c r="P68" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N68" s="4">
+        <v>100</v>
+      </c>
+      <c r="P68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE)),"",VLOOKUP(RANK(Q68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q68" s="4"/>
-      <c r="S68" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q68" s="4">
+        <v>40</v>
+      </c>
+      <c r="S68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE)),"",VLOOKUP(RANK(T68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  score, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T68" s="4"/>
+        <v>-25</v>
+      </c>
+      <c r="T68" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
@@ -4931,171 +4675,175 @@
       <c r="B69" s="4">
         <v>1</v>
       </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="3" t="str">
+      <c r="C69" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE)),"",VLOOKUP(RANK(E69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E69" s="4"/>
-      <c r="G69" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E69" s="4">
+        <v>100</v>
+      </c>
+      <c r="G69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE)),"",VLOOKUP(RANK(H69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H69" s="4"/>
-      <c r="J69" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H69" s="4">
+        <v>40</v>
+      </c>
+      <c r="J69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE)),"",VLOOKUP(RANK(K69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K69" s="4"/>
-      <c r="M69" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K69" s="4">
+        <v>60</v>
+      </c>
+      <c r="M69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE)),"",VLOOKUP(RANK(N69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N69" s="4"/>
-      <c r="P69" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N69" s="4">
+        <v>80</v>
+      </c>
+      <c r="P69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE)),"",VLOOKUP(RANK(Q69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q69" s="4"/>
-      <c r="S69" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q69" s="4">
+        <v>0</v>
+      </c>
+      <c r="S69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE)),"",VLOOKUP(RANK(T69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  score, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T69" s="4"/>
+        <v>-20</v>
+      </c>
+      <c r="T69" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="4"/>
-      <c r="P70" s="4"/>
-      <c r="Q70" s="4"/>
-      <c r="S70" s="4"/>
-      <c r="T70" s="4"/>
+      <c r="A70" s="6"/>
+      <c r="B70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="10"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="1"/>
+      <c r="H70" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J70" s="1"/>
+      <c r="K70" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M70" s="1"/>
+      <c r="N70" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="S70" s="1"/>
+      <c r="T70" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A71" s="6"/>
-      <c r="B71" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71" s="10"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="9" t="s">
-        <v>12</v>
+      <c r="E71" s="11" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
       </c>
       <c r="G71" s="1"/>
-      <c r="H71" s="9" t="s">
-        <v>12</v>
+      <c r="H71" s="11" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
       </c>
       <c r="J71" s="1"/>
-      <c r="K71" s="9" t="s">
-        <v>12</v>
+      <c r="K71" s="11" t="str">
+        <f>J9</f>
+        <v>Justin</v>
       </c>
       <c r="M71" s="1"/>
-      <c r="N71" s="9" t="s">
-        <v>12</v>
+      <c r="N71" s="11" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
       </c>
       <c r="P71" s="1"/>
-      <c r="Q71" s="9" t="s">
-        <v>12</v>
+      <c r="Q71" s="11" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
       </c>
       <c r="S71" s="1"/>
-      <c r="T71" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T71" s="11" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="11" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G72" s="1"/>
-      <c r="H72" s="11" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J72" s="1"/>
-      <c r="K72" s="11" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M72" s="1"/>
-      <c r="N72" s="11" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="11" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S72" s="1"/>
-      <c r="T72" s="11" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="D72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="12">
+        <f>SUM(D10:D69)</f>
+        <v>-100</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="12">
+        <f>SUM(G10:G69)</f>
+        <v>195</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K72" s="12">
+        <f>SUM(J10:J69)</f>
+        <v>187.5</v>
+      </c>
+      <c r="M72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N72" s="12">
+        <f>SUM(M10:M69)</f>
+        <v>315</v>
+      </c>
+      <c r="P72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q72" s="12">
+        <f>SUM(P10:P69)</f>
+        <v>5</v>
+      </c>
+      <c r="S72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T72" s="12">
+        <f>SUM(S10:S69)</f>
+        <v>-602.5</v>
+      </c>
+      <c r="U72" s="1">
+        <f>SUM(E72,H72,K72,N72,Q72,T72)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
-      <c r="D73" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" s="12">
-        <f>SUM(D10:D69)</f>
-        <v>-120</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H73" s="12">
-        <f>SUM(G10:G69)</f>
-        <v>215</v>
-      </c>
-      <c r="J73" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K73" s="12">
-        <f>SUM(J10:J69)</f>
-        <v>232.5</v>
-      </c>
-      <c r="M73" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N73" s="12">
-        <f>SUM(M10:M69)</f>
-        <v>225</v>
-      </c>
-      <c r="P73" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q73" s="12">
-        <f>SUM(P10:P69)</f>
-        <v>-5</v>
-      </c>
-      <c r="S73" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="T73" s="12">
-        <f>SUM(S10:S69)</f>
-        <v>-547.5</v>
-      </c>
-      <c r="U73" s="1">
-        <f>SUM(E73,H73,K73,N73,Q73,T73)</f>
-        <v>0</v>
-      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
@@ -5118,167 +4866,230 @@
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
+    <row r="78" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+      <c r="B78" s="24"/>
+      <c r="C78" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="26"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="28"/>
+      <c r="L78" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="M78" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="N78" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="O78" s="26"/>
+      <c r="P78" s="27"/>
+      <c r="Q78" s="30" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="79" spans="1:21" ht="19" x14ac:dyDescent="0.25">
-      <c r="B79" s="24"/>
-      <c r="C79" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D79" s="26"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="28"/>
-      <c r="L79" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="M79" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="N79" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="O79" s="26"/>
-      <c r="P79" s="27"/>
-      <c r="Q79" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" ht="19" x14ac:dyDescent="0.25">
-      <c r="B80" s="31"/>
-      <c r="C80" s="32" t="s">
+      <c r="B79" s="31"/>
+      <c r="C79" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="D80" s="32" t="s">
+      <c r="D79" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="E80" s="32" t="s">
+      <c r="E79" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="F80" s="32" t="s">
+      <c r="F79" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="G80" s="33" t="s">
+      <c r="G79" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="L80" s="34"/>
-      <c r="M80" s="30"/>
-      <c r="N80" s="32" t="s">
+      <c r="L79" s="34"/>
+      <c r="M79" s="30"/>
+      <c r="N79" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="O80" s="32" t="s">
+      <c r="O79" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="P80" s="32" t="s">
+      <c r="P79" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="Q80" s="30"/>
-    </row>
-    <row r="81" spans="2:18" ht="21" x14ac:dyDescent="0.25">
+      <c r="Q79" s="30"/>
+    </row>
+    <row r="80" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="B80" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1">
+        <v>3</v>
+      </c>
+      <c r="E80" s="1">
+        <v>5</v>
+      </c>
+      <c r="F80" s="1">
+        <v>3</v>
+      </c>
+      <c r="G80" s="1">
+        <f>SUM(C80:F80)</f>
+        <v>11</v>
+      </c>
+      <c r="L80" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="M80" s="12">
+        <f>E72</f>
+        <v>-100</v>
+      </c>
+      <c r="N80" s="36">
+        <v>-120</v>
+      </c>
+      <c r="O80" s="12">
+        <f>G80</f>
+        <v>11</v>
+      </c>
+      <c r="P80" s="12">
+        <f>(-SUM($N$80:$N$85)/SUM($O$80:$O$85))*O80</f>
+        <v>102.85714285714285</v>
+      </c>
+      <c r="Q80" s="12">
+        <f>SUM(M80,N80,P80)</f>
+        <v>-117.14285714285715</v>
+      </c>
+      <c r="R80" s="32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="2:19" ht="21" x14ac:dyDescent="0.25">
       <c r="B81" s="35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C81" s="1">
         <v>0</v>
       </c>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
+      <c r="D81" s="1">
+        <v>3</v>
+      </c>
+      <c r="E81" s="1">
+        <v>10</v>
+      </c>
+      <c r="F81" s="1">
+        <v>3</v>
+      </c>
       <c r="G81" s="1">
-        <f>SUM(C81:F81)</f>
-        <v>0</v>
+        <f t="shared" ref="G81:G85" si="0">SUM(C81:F81)</f>
+        <v>16</v>
       </c>
       <c r="L81" s="35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M81" s="12">
-        <f>E73</f>
-        <v>-120</v>
+        <f>H72</f>
+        <v>195</v>
       </c>
       <c r="N81" s="36">
         <v>-120</v>
       </c>
       <c r="O81" s="12">
-        <f>G81</f>
-        <v>0</v>
+        <f t="shared" ref="O81:O84" si="1">G81</f>
+        <v>16</v>
       </c>
       <c r="P81" s="12">
-        <f>(-SUM($N$81:$N$86)/SUM($O$81:$O$86))*O81</f>
-        <v>0</v>
+        <f t="shared" ref="P81:P86" si="2">(-SUM($N$80:$N$85)/SUM($O$80:$O$85))*O81</f>
+        <v>149.6103896103896</v>
       </c>
       <c r="Q81" s="12">
-        <f>SUM(M81,N81,P81)</f>
-        <v>-240</v>
+        <f t="shared" ref="Q81:Q84" si="3">SUM(M81,N81,P81)</f>
+        <v>224.6103896103896</v>
       </c>
       <c r="R81" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="S81" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="2:19" ht="21" x14ac:dyDescent="0.25">
+      <c r="B82" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="1">
+        <v>10</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="2:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="B82" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" s="1">
-        <v>0</v>
-      </c>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
+      <c r="F82" s="1">
+        <v>3</v>
+      </c>
       <c r="G82" s="1">
-        <f t="shared" ref="G82:G86" si="0">SUM(C82:F82)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="L82" s="35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M82" s="12">
-        <f>H73</f>
-        <v>215</v>
+        <f>K72</f>
+        <v>187.5</v>
       </c>
       <c r="N82" s="36">
         <v>-120</v>
       </c>
       <c r="O82" s="12">
-        <f t="shared" ref="O82:O85" si="1">G82</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="P82" s="12">
-        <f t="shared" ref="P82:P86" si="2">(-SUM($N$81:$N$86)/SUM($O$81:$O$86))*O82</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>168.3116883116883</v>
       </c>
       <c r="Q82" s="12">
-        <f t="shared" ref="Q82:Q85" si="3">SUM(M82,N82,P82)</f>
-        <v>95</v>
+        <f t="shared" si="3"/>
+        <v>235.8116883116883</v>
       </c>
       <c r="R82" s="32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="2:18" ht="21" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="S82" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="2:19" ht="21" x14ac:dyDescent="0.25">
       <c r="B83" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="1">
         <v>7</v>
       </c>
-      <c r="C83" s="1">
-        <v>10</v>
-      </c>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>3</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
       <c r="G83" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L83" s="35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M83" s="12">
-        <f>K73</f>
-        <v>232.5</v>
+        <f>N72</f>
+        <v>315</v>
       </c>
       <c r="N83" s="36">
         <v>-120</v>
@@ -5289,149 +5100,124 @@
       </c>
       <c r="P83" s="12">
         <f t="shared" si="2"/>
-        <v>313.04347826086956</v>
+        <v>93.506493506493499</v>
       </c>
       <c r="Q83" s="12">
         <f t="shared" si="3"/>
-        <v>425.54347826086956</v>
+        <v>288.50649350649348</v>
       </c>
       <c r="R83" s="32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="2:18" ht="21" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="S83" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84" spans="2:19" ht="21" x14ac:dyDescent="0.25">
       <c r="B84" s="35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C84" s="1">
-        <v>7</v>
-      </c>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>3</v>
+      </c>
       <c r="G84" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L84" s="35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M84" s="12">
-        <f>N73</f>
-        <v>225</v>
+        <f>Q72</f>
+        <v>5</v>
       </c>
       <c r="N84" s="36">
         <v>-120</v>
       </c>
       <c r="O84" s="12">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P84" s="12">
         <f t="shared" si="2"/>
-        <v>219.13043478260869</v>
+        <v>56.103896103896105</v>
       </c>
       <c r="Q84" s="12">
         <f t="shared" si="3"/>
-        <v>324.13043478260869</v>
+        <v>-58.896103896103895</v>
       </c>
       <c r="R84" s="32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="2:18" ht="21" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="2:19" ht="21" x14ac:dyDescent="0.25">
       <c r="B85" s="35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C85" s="1">
         <v>3</v>
       </c>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
+      <c r="D85" s="1">
+        <v>3</v>
+      </c>
+      <c r="E85" s="1">
+        <v>7</v>
+      </c>
+      <c r="F85" s="1">
+        <v>3</v>
+      </c>
       <c r="G85" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="L85" s="35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M85" s="12">
-        <f>Q73</f>
-        <v>-5</v>
+        <f>T72</f>
+        <v>-602.5</v>
       </c>
       <c r="N85" s="36">
         <v>-120</v>
       </c>
       <c r="O85" s="12">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" ref="O85" si="4">G85</f>
+        <v>16</v>
       </c>
       <c r="P85" s="12">
         <f t="shared" si="2"/>
-        <v>93.913043478260875</v>
+        <v>149.6103896103896</v>
       </c>
       <c r="Q85" s="12">
-        <f t="shared" si="3"/>
-        <v>-31.086956521739125</v>
+        <f t="shared" ref="Q85" si="5">SUM(M85,N85,P85)</f>
+        <v>-572.88961038961043</v>
       </c>
       <c r="R85" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="2:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="B86" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="1">
-        <v>3</v>
-      </c>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L86" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="M86" s="12">
-        <f>T73</f>
-        <v>-547.5</v>
-      </c>
-      <c r="N86" s="36">
-        <v>-120</v>
-      </c>
-      <c r="O86" s="12">
-        <f t="shared" ref="O86" si="4">G86</f>
-        <v>3</v>
-      </c>
-      <c r="P86" s="12">
-        <f t="shared" si="2"/>
-        <v>93.913043478260875</v>
-      </c>
-      <c r="Q86" s="12">
-        <f t="shared" ref="Q86" si="5">SUM(M86,N86,P86)</f>
-        <v>-573.58695652173913</v>
-      </c>
-      <c r="R86" s="32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="2:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="Q87" s="37">
-        <f>SUM(Q81:Q86)</f>
+    </row>
+    <row r="86" spans="2:19" ht="21" x14ac:dyDescent="0.25">
+      <c r="Q86" s="37">
+        <f>SUM(Q80:Q85)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C79:F79"/>
-    <mergeCell ref="L79:L80"/>
-    <mergeCell ref="M79:M80"/>
-    <mergeCell ref="N79:P79"/>
-    <mergeCell ref="Q79:Q80"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="L78:L79"/>
+    <mergeCell ref="M78:M79"/>
+    <mergeCell ref="N78:P78"/>
+    <mergeCell ref="Q78:Q79"/>
     <mergeCell ref="I2:O6"/>
     <mergeCell ref="S8:T8"/>
     <mergeCell ref="D8:E8"/>
@@ -5440,113 +5226,113 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E73">
-    <cfRule type="cellIs" dxfId="59" priority="61" operator="lessThan">
+  <conditionalFormatting sqref="E72">
+    <cfRule type="cellIs" dxfId="29" priority="61" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="63" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K73">
-    <cfRule type="cellIs" dxfId="56" priority="25" operator="lessThan">
+  <conditionalFormatting sqref="K72">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H73">
-    <cfRule type="cellIs" dxfId="53" priority="28" operator="lessThan">
+  <conditionalFormatting sqref="H72">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N73">
-    <cfRule type="cellIs" dxfId="50" priority="22" operator="lessThan">
+  <conditionalFormatting sqref="N72">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T73">
-    <cfRule type="cellIs" dxfId="47" priority="13" operator="lessThan">
+  <conditionalFormatting sqref="T72">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q73">
-    <cfRule type="cellIs" dxfId="44" priority="16" operator="lessThan">
+  <conditionalFormatting sqref="Q72">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M81:M85">
-    <cfRule type="cellIs" dxfId="41" priority="10" operator="lessThan">
+  <conditionalFormatting sqref="M80:M84">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q81:Q85">
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="Q80:Q84">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M86">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="M85">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q86">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="Q85">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5556,16 +5342,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8336F3D9-B2DA-B14A-BEAC-3FAB2279E4CE}">
-  <dimension ref="F17:J33"/>
+  <dimension ref="F17:J60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E15" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView showGridLines="0" topLeftCell="D26" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="37.6640625" bestFit="1" customWidth="1"/>
@@ -5702,6 +5488,237 @@
         <v>8</v>
       </c>
     </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F36" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F40" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F45" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F47" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="H49" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H50" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F51" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F54" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F56" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F58" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F59" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F60" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="I19:I20"/>

</xml_diff>